<commit_message>
BABY9-3: Add PediaSUre food item and Nutriets.
</commit_message>
<xml_diff>
--- a/src/main/resources/FFQRDatabase.xlsx
+++ b/src/main/resources/FFQRDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcot/Documents/tmp/FIU/SP/Baby-feed/src/ffq-food-item-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8965056E-76BB-400A-9264-B4F4545BF11B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C6E35B-93F4-5342-BA6B-56BAA0EF8650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="299">
   <si>
     <t>Foods 1 oz</t>
   </si>
@@ -916,6 +916,12 @@
   <si>
     <t>pancrefi</t>
   </si>
+  <si>
+    <t>PediaSure (Grow &amp; Gain Shakes)</t>
+  </si>
+  <si>
+    <t>pds</t>
+  </si>
 </sst>
 </file>
 
@@ -1300,183 +1306,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:GI85"/>
+  <dimension ref="A1:GI86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="47.75" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
+    <col min="1" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.625" customWidth="1"/>
-    <col min="9" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="10" width="10.125" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="34.875" customWidth="1"/>
-    <col min="13" max="13" width="41.375" customWidth="1"/>
-    <col min="14" max="14" width="37.625" customWidth="1"/>
-    <col min="15" max="15" width="10.75" customWidth="1"/>
-    <col min="16" max="16" width="11.75" customWidth="1"/>
-    <col min="17" max="17" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" customWidth="1"/>
+    <col min="13" max="13" width="41.33203125" customWidth="1"/>
+    <col min="14" max="14" width="37.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="10.125" customWidth="1"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="19.625" customWidth="1"/>
-    <col min="23" max="23" width="21.75" customWidth="1"/>
-    <col min="24" max="24" width="23.125" customWidth="1"/>
-    <col min="25" max="25" width="9.625" customWidth="1"/>
-    <col min="26" max="26" width="25.125" customWidth="1"/>
-    <col min="27" max="27" width="29.125" customWidth="1"/>
-    <col min="28" max="28" width="12.125" customWidth="1"/>
-    <col min="29" max="29" width="14.625" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" customWidth="1"/>
+    <col min="24" max="24" width="23.1640625" customWidth="1"/>
+    <col min="25" max="25" width="9.6640625" customWidth="1"/>
+    <col min="26" max="26" width="45.5" customWidth="1"/>
+    <col min="27" max="27" width="29.1640625" customWidth="1"/>
+    <col min="28" max="28" width="12.1640625" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" customWidth="1"/>
     <col min="30" max="30" width="27.5" customWidth="1"/>
     <col min="31" max="31" width="32" customWidth="1"/>
-    <col min="32" max="32" width="16.75" customWidth="1"/>
-    <col min="33" max="34" width="17.125" customWidth="1"/>
-    <col min="35" max="35" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="41" width="14.625" customWidth="1"/>
-    <col min="42" max="42" width="16.375" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" customWidth="1"/>
+    <col min="33" max="34" width="17.1640625" customWidth="1"/>
+    <col min="35" max="35" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="14.6640625" customWidth="1"/>
+    <col min="39" max="39" width="26.33203125" customWidth="1"/>
+    <col min="40" max="40" width="25.6640625" customWidth="1"/>
+    <col min="41" max="41" width="33.33203125" customWidth="1"/>
+    <col min="42" max="42" width="16.33203125" customWidth="1"/>
     <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="11.75" customWidth="1"/>
+    <col min="44" max="44" width="11.6640625" customWidth="1"/>
     <col min="45" max="45" width="15.5" customWidth="1"/>
-    <col min="46" max="46" width="15.125" customWidth="1"/>
-    <col min="47" max="48" width="8.625" customWidth="1"/>
-    <col min="49" max="49" width="11.375" customWidth="1"/>
-    <col min="50" max="50" width="14.125" customWidth="1"/>
-    <col min="51" max="51" width="11.625" customWidth="1"/>
-    <col min="52" max="52" width="14.125" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" customWidth="1"/>
+    <col min="47" max="48" width="8.6640625" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" customWidth="1"/>
+    <col min="50" max="50" width="14.1640625" customWidth="1"/>
+    <col min="51" max="51" width="11.6640625" customWidth="1"/>
+    <col min="52" max="52" width="14.1640625" customWidth="1"/>
     <col min="53" max="53" width="22" customWidth="1"/>
-    <col min="54" max="54" width="22.125" customWidth="1"/>
+    <col min="54" max="54" width="22.1640625" customWidth="1"/>
     <col min="55" max="55" width="22.5" customWidth="1"/>
     <col min="56" max="56" width="22" customWidth="1"/>
-    <col min="57" max="57" width="21.625" customWidth="1"/>
-    <col min="58" max="59" width="23.625" customWidth="1"/>
-    <col min="60" max="60" width="24.375" customWidth="1"/>
+    <col min="57" max="57" width="21.6640625" customWidth="1"/>
+    <col min="58" max="59" width="23.6640625" customWidth="1"/>
+    <col min="60" max="60" width="24.33203125" customWidth="1"/>
     <col min="61" max="61" width="22.5" customWidth="1"/>
-    <col min="62" max="62" width="24.625" customWidth="1"/>
-    <col min="63" max="63" width="23.625" customWidth="1"/>
-    <col min="64" max="64" width="28.375" customWidth="1"/>
+    <col min="62" max="62" width="24.6640625" customWidth="1"/>
+    <col min="63" max="63" width="23.6640625" customWidth="1"/>
+    <col min="64" max="64" width="28.33203125" customWidth="1"/>
     <col min="65" max="65" width="28.5" customWidth="1"/>
-    <col min="66" max="66" width="22.75" customWidth="1"/>
-    <col min="67" max="67" width="26.125" customWidth="1"/>
+    <col min="66" max="66" width="22.6640625" customWidth="1"/>
+    <col min="67" max="67" width="26.1640625" customWidth="1"/>
     <col min="68" max="68" width="24" customWidth="1"/>
-    <col min="69" max="69" width="24.375" customWidth="1"/>
-    <col min="70" max="70" width="25.625" customWidth="1"/>
+    <col min="69" max="69" width="24.33203125" customWidth="1"/>
+    <col min="70" max="70" width="25.6640625" customWidth="1"/>
     <col min="71" max="71" width="26" customWidth="1"/>
-    <col min="72" max="72" width="28.375" customWidth="1"/>
-    <col min="73" max="73" width="38.625" customWidth="1"/>
-    <col min="74" max="74" width="39.625" customWidth="1"/>
-    <col min="75" max="75" width="38.75" customWidth="1"/>
-    <col min="76" max="76" width="13.75" customWidth="1"/>
-    <col min="77" max="77" width="12.375" customWidth="1"/>
-    <col min="78" max="78" width="12.125" customWidth="1"/>
-    <col min="79" max="79" width="10.125" customWidth="1"/>
-    <col min="80" max="80" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="13.625" customWidth="1"/>
-    <col min="82" max="82" width="9.625" customWidth="1"/>
-    <col min="83" max="83" width="15.75" customWidth="1"/>
-    <col min="84" max="84" width="10.75" customWidth="1"/>
-    <col min="85" max="85" width="8.75" customWidth="1"/>
-    <col min="86" max="86" width="10.75" customWidth="1"/>
-    <col min="87" max="87" width="11.125" customWidth="1"/>
-    <col min="88" max="88" width="10.125" customWidth="1"/>
+    <col min="72" max="72" width="28.33203125" customWidth="1"/>
+    <col min="73" max="73" width="38.6640625" customWidth="1"/>
+    <col min="74" max="74" width="39.6640625" customWidth="1"/>
+    <col min="75" max="75" width="38.6640625" customWidth="1"/>
+    <col min="76" max="76" width="13.6640625" customWidth="1"/>
+    <col min="77" max="77" width="12.33203125" customWidth="1"/>
+    <col min="78" max="78" width="12.1640625" customWidth="1"/>
+    <col min="79" max="79" width="10.1640625" customWidth="1"/>
+    <col min="80" max="80" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.6640625" customWidth="1"/>
+    <col min="82" max="82" width="9.6640625" customWidth="1"/>
+    <col min="83" max="83" width="15.6640625" customWidth="1"/>
+    <col min="84" max="84" width="10.6640625" customWidth="1"/>
+    <col min="85" max="85" width="8.6640625" customWidth="1"/>
+    <col min="86" max="86" width="10.6640625" customWidth="1"/>
+    <col min="87" max="87" width="11.1640625" customWidth="1"/>
+    <col min="88" max="88" width="10.1640625" customWidth="1"/>
     <col min="89" max="89" width="15" customWidth="1"/>
-    <col min="90" max="90" width="15.625" customWidth="1"/>
-    <col min="91" max="91" width="9.75" customWidth="1"/>
-    <col min="92" max="92" width="9.625" customWidth="1"/>
+    <col min="90" max="90" width="49.33203125" customWidth="1"/>
+    <col min="91" max="91" width="9.6640625" customWidth="1"/>
+    <col min="92" max="92" width="22.6640625" customWidth="1"/>
     <col min="93" max="93" width="9" customWidth="1"/>
-    <col min="94" max="94" width="14.625" customWidth="1"/>
-    <col min="95" max="95" width="13.625" customWidth="1"/>
-    <col min="96" max="96" width="12.125" customWidth="1"/>
+    <col min="94" max="94" width="14.6640625" customWidth="1"/>
+    <col min="95" max="95" width="13.6640625" customWidth="1"/>
+    <col min="96" max="96" width="12.1640625" customWidth="1"/>
     <col min="97" max="97" width="15" customWidth="1"/>
-    <col min="98" max="98" width="14.625" customWidth="1"/>
-    <col min="99" max="99" width="20.625" customWidth="1"/>
+    <col min="98" max="98" width="14.6640625" customWidth="1"/>
+    <col min="99" max="99" width="20.6640625" customWidth="1"/>
     <col min="100" max="100" width="19" customWidth="1"/>
-    <col min="101" max="101" width="6.625" customWidth="1"/>
+    <col min="101" max="101" width="6.6640625" customWidth="1"/>
     <col min="102" max="102" width="9" customWidth="1"/>
     <col min="103" max="103" width="17.5" customWidth="1"/>
-    <col min="104" max="104" width="26.75" customWidth="1"/>
-    <col min="105" max="105" width="21.375" customWidth="1"/>
+    <col min="104" max="104" width="26.6640625" customWidth="1"/>
+    <col min="105" max="105" width="21.33203125" customWidth="1"/>
     <col min="106" max="106" width="21.5" customWidth="1"/>
     <col min="107" max="107" width="18" customWidth="1"/>
     <col min="108" max="108" width="20" customWidth="1"/>
-    <col min="109" max="109" width="19.375" customWidth="1"/>
-    <col min="110" max="110" width="35.375" customWidth="1"/>
-    <col min="111" max="111" width="36.75" customWidth="1"/>
-    <col min="112" max="112" width="45.625" customWidth="1"/>
-    <col min="113" max="113" width="36.125" customWidth="1"/>
+    <col min="109" max="109" width="19.33203125" customWidth="1"/>
+    <col min="110" max="110" width="35.33203125" customWidth="1"/>
+    <col min="111" max="111" width="36.6640625" customWidth="1"/>
+    <col min="112" max="112" width="45.6640625" customWidth="1"/>
+    <col min="113" max="113" width="36.1640625" customWidth="1"/>
     <col min="114" max="114" width="39" customWidth="1"/>
     <col min="115" max="115" width="36.5" customWidth="1"/>
-    <col min="116" max="116" width="31.125" customWidth="1"/>
-    <col min="117" max="117" width="42.125" customWidth="1"/>
-    <col min="118" max="118" width="43.375" customWidth="1"/>
-    <col min="119" max="119" width="46.75" customWidth="1"/>
-    <col min="120" max="120" width="23.375" customWidth="1"/>
-    <col min="121" max="121" width="14.375" customWidth="1"/>
+    <col min="116" max="116" width="31.1640625" customWidth="1"/>
+    <col min="117" max="117" width="42.1640625" customWidth="1"/>
+    <col min="118" max="118" width="43.33203125" customWidth="1"/>
+    <col min="119" max="119" width="46.6640625" customWidth="1"/>
+    <col min="120" max="120" width="23.33203125" customWidth="1"/>
+    <col min="121" max="121" width="14.33203125" customWidth="1"/>
     <col min="122" max="122" width="29" customWidth="1"/>
-    <col min="123" max="123" width="30.125" customWidth="1"/>
+    <col min="123" max="123" width="30.1640625" customWidth="1"/>
     <col min="124" max="124" width="30" customWidth="1"/>
-    <col min="125" max="125" width="53.125" customWidth="1"/>
+    <col min="125" max="125" width="53.1640625" customWidth="1"/>
     <col min="126" max="126" width="10" customWidth="1"/>
-    <col min="127" max="127" width="21.375" customWidth="1"/>
-    <col min="128" max="128" width="14.125" customWidth="1"/>
+    <col min="127" max="127" width="21.33203125" customWidth="1"/>
+    <col min="128" max="128" width="14.1640625" customWidth="1"/>
     <col min="129" max="129" width="21.5" customWidth="1"/>
-    <col min="130" max="130" width="15.125" customWidth="1"/>
+    <col min="130" max="130" width="15.1640625" customWidth="1"/>
     <col min="131" max="131" width="12.5" customWidth="1"/>
-    <col min="132" max="132" width="28.125" customWidth="1"/>
-    <col min="133" max="133" width="29.75" customWidth="1"/>
+    <col min="132" max="132" width="28.1640625" customWidth="1"/>
+    <col min="133" max="133" width="29.6640625" customWidth="1"/>
     <col min="134" max="134" width="12.5" customWidth="1"/>
-    <col min="135" max="135" width="13.375" customWidth="1"/>
-    <col min="136" max="136" width="12.625" customWidth="1"/>
-    <col min="137" max="137" width="15.125" customWidth="1"/>
-    <col min="138" max="138" width="15.625" customWidth="1"/>
-    <col min="139" max="139" width="17.625" customWidth="1"/>
-    <col min="140" max="140" width="40.625" customWidth="1"/>
-    <col min="141" max="141" width="24.625" customWidth="1"/>
+    <col min="135" max="135" width="13.33203125" customWidth="1"/>
+    <col min="136" max="136" width="12.6640625" customWidth="1"/>
+    <col min="137" max="137" width="15.1640625" customWidth="1"/>
+    <col min="138" max="138" width="15.6640625" customWidth="1"/>
+    <col min="139" max="139" width="17.6640625" customWidth="1"/>
+    <col min="140" max="140" width="40.6640625" customWidth="1"/>
+    <col min="141" max="141" width="24.6640625" customWidth="1"/>
     <col min="142" max="142" width="13.5" customWidth="1"/>
-    <col min="143" max="143" width="24.125" customWidth="1"/>
+    <col min="143" max="143" width="24.1640625" customWidth="1"/>
     <col min="144" max="144" width="31" customWidth="1"/>
-    <col min="145" max="145" width="29.625" customWidth="1"/>
+    <col min="145" max="145" width="29.6640625" customWidth="1"/>
     <col min="146" max="146" width="30.5" customWidth="1"/>
     <col min="147" max="147" width="29" customWidth="1"/>
-    <col min="148" max="149" width="11.625" customWidth="1"/>
-    <col min="150" max="150" width="11.75" customWidth="1"/>
+    <col min="148" max="150" width="11.6640625" customWidth="1"/>
     <col min="151" max="151" width="10" customWidth="1"/>
-    <col min="152" max="152" width="9.75" customWidth="1"/>
+    <col min="152" max="152" width="9.6640625" customWidth="1"/>
     <col min="153" max="153" width="10" customWidth="1"/>
     <col min="154" max="154" width="10.5" customWidth="1"/>
     <col min="155" max="155" width="11.5" customWidth="1"/>
-    <col min="156" max="156" width="9.125" customWidth="1"/>
+    <col min="156" max="156" width="9.1640625" customWidth="1"/>
     <col min="157" max="157" width="10.5" customWidth="1"/>
-    <col min="158" max="158" width="9.125" customWidth="1"/>
-    <col min="159" max="159" width="11.125" customWidth="1"/>
-    <col min="160" max="160" width="39.125" customWidth="1"/>
-    <col min="161" max="161" width="19.125" customWidth="1"/>
-    <col min="162" max="162" width="20.125" customWidth="1"/>
+    <col min="158" max="158" width="9.1640625" customWidth="1"/>
+    <col min="159" max="159" width="11.1640625" customWidth="1"/>
+    <col min="160" max="160" width="39.1640625" customWidth="1"/>
+    <col min="161" max="161" width="19.1640625" customWidth="1"/>
+    <col min="162" max="162" width="20.1640625" customWidth="1"/>
     <col min="163" max="163" width="13" customWidth="1"/>
     <col min="164" max="164" width="29.5" customWidth="1"/>
-    <col min="165" max="165" width="30.125" customWidth="1"/>
-    <col min="166" max="166" width="30.75" customWidth="1"/>
+    <col min="165" max="165" width="30.1640625" customWidth="1"/>
+    <col min="166" max="166" width="30.6640625" customWidth="1"/>
     <col min="167" max="167" width="29" customWidth="1"/>
-    <col min="168" max="168" width="30.375" customWidth="1"/>
-    <col min="169" max="169" width="31.125" customWidth="1"/>
-    <col min="170" max="170" width="39.625" customWidth="1"/>
-    <col min="171" max="171" width="11.625" customWidth="1"/>
-    <col min="172" max="191" width="8.75" customWidth="1"/>
+    <col min="168" max="168" width="30.33203125" customWidth="1"/>
+    <col min="169" max="169" width="31.1640625" customWidth="1"/>
+    <col min="170" max="170" width="39.6640625" customWidth="1"/>
+    <col min="171" max="171" width="11.6640625" customWidth="1"/>
+    <col min="172" max="191" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +1935,7 @@
       <c r="GH1" s="3"/>
       <c r="GI1" s="3"/>
     </row>
-    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -2378,7 +2386,7 @@
       <c r="GH2" s="4"/>
       <c r="GI2" s="4"/>
     </row>
-    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>129</v>
       </c>
@@ -2829,7 +2837,7 @@
       <c r="GH3" s="4"/>
       <c r="GI3" s="4"/>
     </row>
-    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>290</v>
       </c>
@@ -3280,7 +3288,7 @@
       <c r="GH4" s="4"/>
       <c r="GI4" s="4"/>
     </row>
-    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>130</v>
       </c>
@@ -3731,7 +3739,7 @@
       <c r="GH5" s="4"/>
       <c r="GI5" s="4"/>
     </row>
-    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>131</v>
       </c>
@@ -4182,7 +4190,7 @@
       <c r="GH6" s="4"/>
       <c r="GI6" s="4"/>
     </row>
-    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -4633,7 +4641,7 @@
       <c r="GH7" s="4"/>
       <c r="GI7" s="4"/>
     </row>
-    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>133</v>
       </c>
@@ -5084,7 +5092,7 @@
       <c r="GH8" s="4"/>
       <c r="GI8" s="4"/>
     </row>
-    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>134</v>
       </c>
@@ -5535,7 +5543,7 @@
       <c r="GH9" s="4"/>
       <c r="GI9" s="4"/>
     </row>
-    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>135</v>
       </c>
@@ -5986,7 +5994,7 @@
       <c r="GH10" s="4"/>
       <c r="GI10" s="4"/>
     </row>
-    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>136</v>
       </c>
@@ -6437,7 +6445,7 @@
       <c r="GH11" s="4"/>
       <c r="GI11" s="4"/>
     </row>
-    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>137</v>
       </c>
@@ -6888,7 +6896,7 @@
       <c r="GH12" s="4"/>
       <c r="GI12" s="4"/>
     </row>
-    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>138</v>
       </c>
@@ -7339,7 +7347,7 @@
       <c r="GH13" s="4"/>
       <c r="GI13" s="4"/>
     </row>
-    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>139</v>
       </c>
@@ -7790,7 +7798,7 @@
       <c r="GH14" s="4"/>
       <c r="GI14" s="4"/>
     </row>
-    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>140</v>
       </c>
@@ -8241,7 +8249,7 @@
       <c r="GH15" s="4"/>
       <c r="GI15" s="4"/>
     </row>
-    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>141</v>
       </c>
@@ -8692,7 +8700,7 @@
       <c r="GH16" s="4"/>
       <c r="GI16" s="4"/>
     </row>
-    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>142</v>
       </c>
@@ -9143,7 +9151,7 @@
       <c r="GH17" s="4"/>
       <c r="GI17" s="4"/>
     </row>
-    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>143</v>
       </c>
@@ -9594,7 +9602,7 @@
       <c r="GH18" s="4"/>
       <c r="GI18" s="4"/>
     </row>
-    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>144</v>
       </c>
@@ -10045,7 +10053,7 @@
       <c r="GH19" s="4"/>
       <c r="GI19" s="4"/>
     </row>
-    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>145</v>
       </c>
@@ -10496,7 +10504,7 @@
       <c r="GH20" s="4"/>
       <c r="GI20" s="4"/>
     </row>
-    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>146</v>
       </c>
@@ -10947,7 +10955,7 @@
       <c r="GH21" s="4"/>
       <c r="GI21" s="4"/>
     </row>
-    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>147</v>
       </c>
@@ -11398,7 +11406,7 @@
       <c r="GH22" s="4"/>
       <c r="GI22" s="4"/>
     </row>
-    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>148</v>
       </c>
@@ -11849,7 +11857,7 @@
       <c r="GH23" s="4"/>
       <c r="GI23" s="4"/>
     </row>
-    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>149</v>
       </c>
@@ -12300,7 +12308,7 @@
       <c r="GH24" s="4"/>
       <c r="GI24" s="4"/>
     </row>
-    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>150</v>
       </c>
@@ -12751,7 +12759,7 @@
       <c r="GH25" s="4"/>
       <c r="GI25" s="4"/>
     </row>
-    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>151</v>
       </c>
@@ -13202,7 +13210,7 @@
       <c r="GH26" s="4"/>
       <c r="GI26" s="4"/>
     </row>
-    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>152</v>
       </c>
@@ -13653,7 +13661,7 @@
       <c r="GH27" s="4"/>
       <c r="GI27" s="4"/>
     </row>
-    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>153</v>
       </c>
@@ -14104,7 +14112,7 @@
       <c r="GH28" s="4"/>
       <c r="GI28" s="4"/>
     </row>
-    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>154</v>
       </c>
@@ -14555,7 +14563,7 @@
       <c r="GH29" s="4"/>
       <c r="GI29" s="4"/>
     </row>
-    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>291</v>
       </c>
@@ -15006,7 +15014,7 @@
       <c r="GH30" s="4"/>
       <c r="GI30" s="4"/>
     </row>
-    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>292</v>
       </c>
@@ -15457,7 +15465,7 @@
       <c r="GH31" s="4"/>
       <c r="GI31" s="4"/>
     </row>
-    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>293</v>
       </c>
@@ -15908,7 +15916,7 @@
       <c r="GH32" s="4"/>
       <c r="GI32" s="4"/>
     </row>
-    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>155</v>
       </c>
@@ -16359,7 +16367,7 @@
       <c r="GH33" s="4"/>
       <c r="GI33" s="4"/>
     </row>
-    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>156</v>
       </c>
@@ -16810,7 +16818,7 @@
       <c r="GH34" s="4"/>
       <c r="GI34" s="4"/>
     </row>
-    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>157</v>
       </c>
@@ -17261,7 +17269,7 @@
       <c r="GH35" s="4"/>
       <c r="GI35" s="4"/>
     </row>
-    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>158</v>
       </c>
@@ -17712,7 +17720,7 @@
       <c r="GH36" s="4"/>
       <c r="GI36" s="4"/>
     </row>
-    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>159</v>
       </c>
@@ -18163,7 +18171,7 @@
       <c r="GH37" s="4"/>
       <c r="GI37" s="4"/>
     </row>
-    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>160</v>
       </c>
@@ -18614,7 +18622,7 @@
       <c r="GH38" s="4"/>
       <c r="GI38" s="4"/>
     </row>
-    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>161</v>
       </c>
@@ -19065,7 +19073,7 @@
       <c r="GH39" s="4"/>
       <c r="GI39" s="4"/>
     </row>
-    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>162</v>
       </c>
@@ -19516,7 +19524,7 @@
       <c r="GH40" s="4"/>
       <c r="GI40" s="4"/>
     </row>
-    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>163</v>
       </c>
@@ -19967,7 +19975,7 @@
       <c r="GH41" s="4"/>
       <c r="GI41" s="4"/>
     </row>
-    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>164</v>
       </c>
@@ -20418,7 +20426,7 @@
       <c r="GH42" s="4"/>
       <c r="GI42" s="4"/>
     </row>
-    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>165</v>
       </c>
@@ -20869,7 +20877,7 @@
       <c r="GH43" s="4"/>
       <c r="GI43" s="4"/>
     </row>
-    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>166</v>
       </c>
@@ -21320,7 +21328,7 @@
       <c r="GH44" s="4"/>
       <c r="GI44" s="4"/>
     </row>
-    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>167</v>
       </c>
@@ -21771,7 +21779,7 @@
       <c r="GH45" s="4"/>
       <c r="GI45" s="4"/>
     </row>
-    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>168</v>
       </c>
@@ -22222,7 +22230,7 @@
       <c r="GH46" s="4"/>
       <c r="GI46" s="4"/>
     </row>
-    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>169</v>
       </c>
@@ -22673,7 +22681,7 @@
       <c r="GH47" s="4"/>
       <c r="GI47" s="4"/>
     </row>
-    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>170</v>
       </c>
@@ -23124,7 +23132,7 @@
       <c r="GH48" s="4"/>
       <c r="GI48" s="4"/>
     </row>
-    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>171</v>
       </c>
@@ -23575,7 +23583,7 @@
       <c r="GH49" s="4"/>
       <c r="GI49" s="4"/>
     </row>
-    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>172</v>
       </c>
@@ -24026,7 +24034,7 @@
       <c r="GH50" s="4"/>
       <c r="GI50" s="4"/>
     </row>
-    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>173</v>
       </c>
@@ -24477,7 +24485,7 @@
       <c r="GH51" s="4"/>
       <c r="GI51" s="4"/>
     </row>
-    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>174</v>
       </c>
@@ -24928,7 +24936,7 @@
       <c r="GH52" s="4"/>
       <c r="GI52" s="4"/>
     </row>
-    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>175</v>
       </c>
@@ -25379,7 +25387,7 @@
       <c r="GH53" s="4"/>
       <c r="GI53" s="4"/>
     </row>
-    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>176</v>
       </c>
@@ -25830,7 +25838,7 @@
       <c r="GH54" s="4"/>
       <c r="GI54" s="4"/>
     </row>
-    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>177</v>
       </c>
@@ -26281,7 +26289,7 @@
       <c r="GH55" s="4"/>
       <c r="GI55" s="4"/>
     </row>
-    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>178</v>
       </c>
@@ -26732,7 +26740,7 @@
       <c r="GH56" s="4"/>
       <c r="GI56" s="4"/>
     </row>
-    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>179</v>
       </c>
@@ -27183,7 +27191,7 @@
       <c r="GH57" s="4"/>
       <c r="GI57" s="4"/>
     </row>
-    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>180</v>
       </c>
@@ -27634,7 +27642,7 @@
       <c r="GH58" s="4"/>
       <c r="GI58" s="4"/>
     </row>
-    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>181</v>
       </c>
@@ -28085,7 +28093,7 @@
       <c r="GH59" s="4"/>
       <c r="GI59" s="4"/>
     </row>
-    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>182</v>
       </c>
@@ -28536,7 +28544,7 @@
       <c r="GH60" s="2"/>
       <c r="GI60" s="2"/>
     </row>
-    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>183</v>
       </c>
@@ -28987,7 +28995,7 @@
       <c r="GH61" s="4"/>
       <c r="GI61" s="4"/>
     </row>
-    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>294</v>
       </c>
@@ -29438,7 +29446,7 @@
       <c r="GH62" s="4"/>
       <c r="GI62" s="4"/>
     </row>
-    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>184</v>
       </c>
@@ -29889,7 +29897,7 @@
       <c r="GH63" s="4"/>
       <c r="GI63" s="4"/>
     </row>
-    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>185</v>
       </c>
@@ -30340,7 +30348,7 @@
       <c r="GH64" s="4"/>
       <c r="GI64" s="4"/>
     </row>
-    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
@@ -30791,7 +30799,7 @@
       <c r="GH65" s="4"/>
       <c r="GI65" s="4"/>
     </row>
-    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>187</v>
       </c>
@@ -31242,7 +31250,7 @@
       <c r="GH66" s="4"/>
       <c r="GI66" s="4"/>
     </row>
-    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>188</v>
       </c>
@@ -31693,7 +31701,7 @@
       <c r="GH67" s="4"/>
       <c r="GI67" s="4"/>
     </row>
-    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -32144,7 +32152,7 @@
       <c r="GH68" s="4"/>
       <c r="GI68" s="4"/>
     </row>
-    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>190</v>
       </c>
@@ -32595,7 +32603,7 @@
       <c r="GH69" s="4"/>
       <c r="GI69" s="4"/>
     </row>
-    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -33046,7 +33054,7 @@
       <c r="GH70" s="4"/>
       <c r="GI70" s="4"/>
     </row>
-    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>192</v>
       </c>
@@ -33497,7 +33505,7 @@
       <c r="GH71" s="4"/>
       <c r="GI71" s="4"/>
     </row>
-    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>193</v>
       </c>
@@ -33948,7 +33956,7 @@
       <c r="GH72" s="4"/>
       <c r="GI72" s="4"/>
     </row>
-    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>194</v>
       </c>
@@ -34399,7 +34407,7 @@
       <c r="GH73" s="4"/>
       <c r="GI73" s="4"/>
     </row>
-    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>195</v>
       </c>
@@ -34850,7 +34858,7 @@
       <c r="GH74" s="4"/>
       <c r="GI74" s="4"/>
     </row>
-    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>196</v>
       </c>
@@ -35301,7 +35309,7 @@
       <c r="GH75" s="4"/>
       <c r="GI75" s="4"/>
     </row>
-    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>197</v>
       </c>
@@ -35752,7 +35760,7 @@
       <c r="GH76" s="4"/>
       <c r="GI76" s="4"/>
     </row>
-    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>198</v>
       </c>
@@ -36203,7 +36211,7 @@
       <c r="GH77" s="4"/>
       <c r="GI77" s="4"/>
     </row>
-    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>199</v>
       </c>
@@ -36654,7 +36662,7 @@
       <c r="GH78" s="4"/>
       <c r="GI78" s="4"/>
     </row>
-    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>200</v>
       </c>
@@ -37105,7 +37113,7 @@
       <c r="GH79" s="4"/>
       <c r="GI79" s="4"/>
     </row>
-    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>201</v>
       </c>
@@ -37556,7 +37564,7 @@
       <c r="GH80" s="4"/>
       <c r="GI80" s="4"/>
     </row>
-    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>202</v>
       </c>
@@ -38007,7 +38015,7 @@
       <c r="GH81" s="4"/>
       <c r="GI81" s="4"/>
     </row>
-    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>203</v>
       </c>
@@ -38458,7 +38466,7 @@
       <c r="GH82" s="4"/>
       <c r="GI82" s="4"/>
     </row>
-    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>204</v>
       </c>
@@ -38909,7 +38917,7 @@
       <c r="GH83" s="4"/>
       <c r="GI83" s="4"/>
     </row>
-    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>205</v>
       </c>
@@ -39360,7 +39368,7 @@
       <c r="GH84" s="4"/>
       <c r="GI84" s="4"/>
     </row>
-    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>206</v>
       </c>
@@ -39747,6 +39755,158 @@
       </c>
       <c r="DY85" s="6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C86" s="2">
+        <v>31</v>
+      </c>
+      <c r="D86" s="2">
+        <v>30</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1.125</v>
+      </c>
+      <c r="F86" s="2">
+        <v>4.125</v>
+      </c>
+      <c r="G86" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="H86" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="I86" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="J86" s="2">
+        <v>0</v>
+      </c>
+      <c r="K86" s="2">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="M86" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="N86" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="O86" s="2">
+        <v>0</v>
+      </c>
+      <c r="P86" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="2">
+        <v>0</v>
+      </c>
+      <c r="R86" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="S86" s="2">
+        <v>0</v>
+      </c>
+      <c r="T86" s="2">
+        <v>0</v>
+      </c>
+      <c r="U86" s="2">
+        <v>0</v>
+      </c>
+      <c r="V86" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="W86" s="2">
+        <v>0</v>
+      </c>
+      <c r="X86" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC86" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AE86" s="2">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="AI86" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ86" s="2">
+        <v>3</v>
+      </c>
+      <c r="AK86" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AL86" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AM86" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="AN86" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="AO86" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AP86" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="AQ86" s="2">
+        <v>0.1875</v>
+      </c>
+      <c r="AR86" s="2">
+        <v>41.25</v>
+      </c>
+      <c r="AS86" s="2">
+        <v>25</v>
+      </c>
+      <c r="AT86" s="2">
+        <v>5</v>
+      </c>
+      <c r="AU86" s="2">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="AV86" s="2">
+        <v>0.1875</v>
+      </c>
+      <c r="AW86" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AX86" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="AY86" s="2">
+        <v>11.25</v>
+      </c>
+      <c r="AZ86" s="2">
+        <v>43.75</v>
+      </c>
+      <c r="CA86" s="2">
+        <v>25</v>
+      </c>
+      <c r="CL86" s="2">
+        <v>18.75</v>
+      </c>
+      <c r="CO86" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="CP86" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="CQ86" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="DT86" s="2">
+        <v>1.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing to see if CHO/folate/panthothenic are showing
</commit_message>
<xml_diff>
--- a/src/main/resources/FFQRDatabase.xlsx
+++ b/src/main/resources/FFQRDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcot/Documents/tmp/FIU/SP/Baby-feed/src/ffq-food-item-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\BabyFeed\ffq-food-item-service\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C6E35B-93F4-5342-BA6B-56BAA0EF8650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C65B34B-3008-4FDA-9DB7-668971D25B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="2325" windowWidth="25380" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,7 @@
     <t>Total Grams</t>
   </si>
   <si>
-    <t>Energy (kcal)</t>
-  </si>
-  <si>
     <t>Total Fat (g)</t>
-  </si>
-  <si>
-    <t>Total Carbohydrate (g)</t>
-  </si>
-  <si>
-    <t>Total Protein (g)</t>
   </si>
   <si>
     <t>Animal Protein (g)</t>
@@ -51,9 +42,6 @@
   </si>
   <si>
     <t>Alcohol (g)</t>
-  </si>
-  <si>
-    <t>Cholesterol (mg)</t>
   </si>
   <si>
     <t>Total Saturated Fatty Acids (SFA) (g)</t>
@@ -140,13 +128,7 @@
     <t>Niacin (vitamin B3) (mg)</t>
   </si>
   <si>
-    <t>Pantothenic Acid (mg)</t>
-  </si>
-  <si>
     <t>Vitamin B-6 (pyridoxine, pyridoxyl, &amp; pyridoxamine) (mg)</t>
-  </si>
-  <si>
-    <t>Total Folate (mcg)</t>
   </si>
   <si>
     <t>Vitamin B-12 (cobalamin) (mcg)</t>
@@ -922,6 +904,24 @@
   <si>
     <t>pds</t>
   </si>
+  <si>
+    <t>Energy (kcal)</t>
+  </si>
+  <si>
+    <t>CHO (g)</t>
+  </si>
+  <si>
+    <t>Vitamin B9 (Folate) (mcg)</t>
+  </si>
+  <si>
+    <t>Cholesterol (mg)</t>
+  </si>
+  <si>
+    <t>Protein (g)</t>
+  </si>
+  <si>
+    <t>Vitamin B5 (Pantothenic acid) (mg)</t>
+  </si>
 </sst>
 </file>
 
@@ -1309,568 +1309,568 @@
   <dimension ref="A1:GI86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
+      <selection pane="bottomRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="1" max="2" width="47.625" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="34.83203125" customWidth="1"/>
-    <col min="13" max="13" width="41.33203125" customWidth="1"/>
-    <col min="14" max="14" width="37.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="14.625" customWidth="1"/>
+    <col min="12" max="12" width="34.875" customWidth="1"/>
+    <col min="13" max="13" width="41.375" customWidth="1"/>
+    <col min="14" max="14" width="37.625" customWidth="1"/>
+    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
+    <col min="17" max="17" width="10.125" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="10.1640625" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" customWidth="1"/>
-    <col min="24" max="24" width="23.1640625" customWidth="1"/>
-    <col min="25" max="25" width="9.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.125" customWidth="1"/>
+    <col min="21" max="21" width="9.125" customWidth="1"/>
+    <col min="22" max="22" width="19.625" customWidth="1"/>
+    <col min="23" max="23" width="21.625" customWidth="1"/>
+    <col min="24" max="24" width="23.125" customWidth="1"/>
+    <col min="25" max="25" width="9.625" customWidth="1"/>
     <col min="26" max="26" width="45.5" customWidth="1"/>
-    <col min="27" max="27" width="29.1640625" customWidth="1"/>
-    <col min="28" max="28" width="12.1640625" customWidth="1"/>
-    <col min="29" max="29" width="14.6640625" customWidth="1"/>
+    <col min="27" max="27" width="29.125" customWidth="1"/>
+    <col min="28" max="28" width="12.125" customWidth="1"/>
+    <col min="29" max="29" width="14.625" customWidth="1"/>
     <col min="30" max="30" width="27.5" customWidth="1"/>
     <col min="31" max="31" width="32" customWidth="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="34" width="17.1640625" customWidth="1"/>
-    <col min="35" max="35" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="14.6640625" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" customWidth="1"/>
-    <col min="40" max="40" width="25.6640625" customWidth="1"/>
-    <col min="41" max="41" width="33.33203125" customWidth="1"/>
-    <col min="42" max="42" width="16.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16.625" customWidth="1"/>
+    <col min="33" max="34" width="17.125" customWidth="1"/>
+    <col min="35" max="35" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="14.625" customWidth="1"/>
+    <col min="39" max="39" width="26.375" customWidth="1"/>
+    <col min="40" max="40" width="25.625" customWidth="1"/>
+    <col min="41" max="41" width="33.375" customWidth="1"/>
+    <col min="42" max="42" width="16.375" customWidth="1"/>
     <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="11.6640625" customWidth="1"/>
+    <col min="44" max="44" width="11.625" customWidth="1"/>
     <col min="45" max="45" width="15.5" customWidth="1"/>
-    <col min="46" max="46" width="15.1640625" customWidth="1"/>
-    <col min="47" max="48" width="8.6640625" customWidth="1"/>
-    <col min="49" max="49" width="11.33203125" customWidth="1"/>
-    <col min="50" max="50" width="14.1640625" customWidth="1"/>
-    <col min="51" max="51" width="11.6640625" customWidth="1"/>
-    <col min="52" max="52" width="14.1640625" customWidth="1"/>
+    <col min="46" max="46" width="15.125" customWidth="1"/>
+    <col min="47" max="48" width="8.625" customWidth="1"/>
+    <col min="49" max="49" width="11.375" customWidth="1"/>
+    <col min="50" max="50" width="14.125" customWidth="1"/>
+    <col min="51" max="51" width="11.625" customWidth="1"/>
+    <col min="52" max="52" width="14.125" customWidth="1"/>
     <col min="53" max="53" width="22" customWidth="1"/>
-    <col min="54" max="54" width="22.1640625" customWidth="1"/>
+    <col min="54" max="54" width="22.125" customWidth="1"/>
     <col min="55" max="55" width="22.5" customWidth="1"/>
     <col min="56" max="56" width="22" customWidth="1"/>
-    <col min="57" max="57" width="21.6640625" customWidth="1"/>
-    <col min="58" max="59" width="23.6640625" customWidth="1"/>
-    <col min="60" max="60" width="24.33203125" customWidth="1"/>
+    <col min="57" max="57" width="21.625" customWidth="1"/>
+    <col min="58" max="59" width="23.625" customWidth="1"/>
+    <col min="60" max="60" width="24.375" customWidth="1"/>
     <col min="61" max="61" width="22.5" customWidth="1"/>
-    <col min="62" max="62" width="24.6640625" customWidth="1"/>
-    <col min="63" max="63" width="23.6640625" customWidth="1"/>
-    <col min="64" max="64" width="28.33203125" customWidth="1"/>
+    <col min="62" max="62" width="24.625" customWidth="1"/>
+    <col min="63" max="63" width="23.625" customWidth="1"/>
+    <col min="64" max="64" width="28.375" customWidth="1"/>
     <col min="65" max="65" width="28.5" customWidth="1"/>
-    <col min="66" max="66" width="22.6640625" customWidth="1"/>
-    <col min="67" max="67" width="26.1640625" customWidth="1"/>
+    <col min="66" max="66" width="22.625" customWidth="1"/>
+    <col min="67" max="67" width="26.125" customWidth="1"/>
     <col min="68" max="68" width="24" customWidth="1"/>
-    <col min="69" max="69" width="24.33203125" customWidth="1"/>
-    <col min="70" max="70" width="25.6640625" customWidth="1"/>
+    <col min="69" max="69" width="24.375" customWidth="1"/>
+    <col min="70" max="70" width="25.625" customWidth="1"/>
     <col min="71" max="71" width="26" customWidth="1"/>
-    <col min="72" max="72" width="28.33203125" customWidth="1"/>
-    <col min="73" max="73" width="38.6640625" customWidth="1"/>
-    <col min="74" max="74" width="39.6640625" customWidth="1"/>
-    <col min="75" max="75" width="38.6640625" customWidth="1"/>
-    <col min="76" max="76" width="13.6640625" customWidth="1"/>
-    <col min="77" max="77" width="12.33203125" customWidth="1"/>
-    <col min="78" max="78" width="12.1640625" customWidth="1"/>
-    <col min="79" max="79" width="10.1640625" customWidth="1"/>
-    <col min="80" max="80" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="13.6640625" customWidth="1"/>
-    <col min="82" max="82" width="9.6640625" customWidth="1"/>
-    <col min="83" max="83" width="15.6640625" customWidth="1"/>
-    <col min="84" max="84" width="10.6640625" customWidth="1"/>
-    <col min="85" max="85" width="8.6640625" customWidth="1"/>
-    <col min="86" max="86" width="10.6640625" customWidth="1"/>
-    <col min="87" max="87" width="11.1640625" customWidth="1"/>
-    <col min="88" max="88" width="10.1640625" customWidth="1"/>
+    <col min="72" max="72" width="28.375" customWidth="1"/>
+    <col min="73" max="73" width="38.625" customWidth="1"/>
+    <col min="74" max="74" width="39.625" customWidth="1"/>
+    <col min="75" max="75" width="38.625" customWidth="1"/>
+    <col min="76" max="76" width="13.625" customWidth="1"/>
+    <col min="77" max="77" width="12.375" customWidth="1"/>
+    <col min="78" max="78" width="12.125" customWidth="1"/>
+    <col min="79" max="79" width="10.125" customWidth="1"/>
+    <col min="80" max="80" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.625" customWidth="1"/>
+    <col min="82" max="82" width="9.625" customWidth="1"/>
+    <col min="83" max="83" width="15.625" customWidth="1"/>
+    <col min="84" max="84" width="10.625" customWidth="1"/>
+    <col min="85" max="85" width="8.625" customWidth="1"/>
+    <col min="86" max="86" width="10.625" customWidth="1"/>
+    <col min="87" max="87" width="11.125" customWidth="1"/>
+    <col min="88" max="88" width="10.125" customWidth="1"/>
     <col min="89" max="89" width="15" customWidth="1"/>
-    <col min="90" max="90" width="49.33203125" customWidth="1"/>
-    <col min="91" max="91" width="9.6640625" customWidth="1"/>
-    <col min="92" max="92" width="22.6640625" customWidth="1"/>
+    <col min="90" max="90" width="49.375" customWidth="1"/>
+    <col min="91" max="91" width="9.625" customWidth="1"/>
+    <col min="92" max="92" width="22.625" customWidth="1"/>
     <col min="93" max="93" width="9" customWidth="1"/>
-    <col min="94" max="94" width="14.6640625" customWidth="1"/>
-    <col min="95" max="95" width="13.6640625" customWidth="1"/>
-    <col min="96" max="96" width="12.1640625" customWidth="1"/>
+    <col min="94" max="94" width="14.625" customWidth="1"/>
+    <col min="95" max="95" width="13.625" customWidth="1"/>
+    <col min="96" max="96" width="12.125" customWidth="1"/>
     <col min="97" max="97" width="15" customWidth="1"/>
-    <col min="98" max="98" width="14.6640625" customWidth="1"/>
-    <col min="99" max="99" width="20.6640625" customWidth="1"/>
+    <col min="98" max="98" width="14.625" customWidth="1"/>
+    <col min="99" max="99" width="20.625" customWidth="1"/>
     <col min="100" max="100" width="19" customWidth="1"/>
-    <col min="101" max="101" width="6.6640625" customWidth="1"/>
+    <col min="101" max="101" width="6.625" customWidth="1"/>
     <col min="102" max="102" width="9" customWidth="1"/>
     <col min="103" max="103" width="17.5" customWidth="1"/>
-    <col min="104" max="104" width="26.6640625" customWidth="1"/>
-    <col min="105" max="105" width="21.33203125" customWidth="1"/>
+    <col min="104" max="104" width="26.625" customWidth="1"/>
+    <col min="105" max="105" width="21.375" customWidth="1"/>
     <col min="106" max="106" width="21.5" customWidth="1"/>
     <col min="107" max="107" width="18" customWidth="1"/>
     <col min="108" max="108" width="20" customWidth="1"/>
-    <col min="109" max="109" width="19.33203125" customWidth="1"/>
-    <col min="110" max="110" width="35.33203125" customWidth="1"/>
-    <col min="111" max="111" width="36.6640625" customWidth="1"/>
-    <col min="112" max="112" width="45.6640625" customWidth="1"/>
-    <col min="113" max="113" width="36.1640625" customWidth="1"/>
+    <col min="109" max="109" width="19.375" customWidth="1"/>
+    <col min="110" max="110" width="35.375" customWidth="1"/>
+    <col min="111" max="111" width="36.625" customWidth="1"/>
+    <col min="112" max="112" width="45.625" customWidth="1"/>
+    <col min="113" max="113" width="36.125" customWidth="1"/>
     <col min="114" max="114" width="39" customWidth="1"/>
     <col min="115" max="115" width="36.5" customWidth="1"/>
-    <col min="116" max="116" width="31.1640625" customWidth="1"/>
-    <col min="117" max="117" width="42.1640625" customWidth="1"/>
-    <col min="118" max="118" width="43.33203125" customWidth="1"/>
-    <col min="119" max="119" width="46.6640625" customWidth="1"/>
-    <col min="120" max="120" width="23.33203125" customWidth="1"/>
-    <col min="121" max="121" width="14.33203125" customWidth="1"/>
+    <col min="116" max="116" width="31.125" customWidth="1"/>
+    <col min="117" max="117" width="42.125" customWidth="1"/>
+    <col min="118" max="118" width="43.375" customWidth="1"/>
+    <col min="119" max="119" width="46.625" customWidth="1"/>
+    <col min="120" max="120" width="23.375" customWidth="1"/>
+    <col min="121" max="121" width="14.375" customWidth="1"/>
     <col min="122" max="122" width="29" customWidth="1"/>
-    <col min="123" max="123" width="30.1640625" customWidth="1"/>
+    <col min="123" max="123" width="30.125" customWidth="1"/>
     <col min="124" max="124" width="30" customWidth="1"/>
-    <col min="125" max="125" width="53.1640625" customWidth="1"/>
+    <col min="125" max="125" width="53.125" customWidth="1"/>
     <col min="126" max="126" width="10" customWidth="1"/>
-    <col min="127" max="127" width="21.33203125" customWidth="1"/>
-    <col min="128" max="128" width="14.1640625" customWidth="1"/>
+    <col min="127" max="127" width="21.375" customWidth="1"/>
+    <col min="128" max="128" width="14.125" customWidth="1"/>
     <col min="129" max="129" width="21.5" customWidth="1"/>
-    <col min="130" max="130" width="15.1640625" customWidth="1"/>
+    <col min="130" max="130" width="15.125" customWidth="1"/>
     <col min="131" max="131" width="12.5" customWidth="1"/>
-    <col min="132" max="132" width="28.1640625" customWidth="1"/>
-    <col min="133" max="133" width="29.6640625" customWidth="1"/>
+    <col min="132" max="132" width="28.125" customWidth="1"/>
+    <col min="133" max="133" width="29.625" customWidth="1"/>
     <col min="134" max="134" width="12.5" customWidth="1"/>
-    <col min="135" max="135" width="13.33203125" customWidth="1"/>
-    <col min="136" max="136" width="12.6640625" customWidth="1"/>
-    <col min="137" max="137" width="15.1640625" customWidth="1"/>
-    <col min="138" max="138" width="15.6640625" customWidth="1"/>
-    <col min="139" max="139" width="17.6640625" customWidth="1"/>
-    <col min="140" max="140" width="40.6640625" customWidth="1"/>
-    <col min="141" max="141" width="24.6640625" customWidth="1"/>
+    <col min="135" max="135" width="13.375" customWidth="1"/>
+    <col min="136" max="136" width="12.625" customWidth="1"/>
+    <col min="137" max="137" width="15.125" customWidth="1"/>
+    <col min="138" max="138" width="15.625" customWidth="1"/>
+    <col min="139" max="139" width="17.625" customWidth="1"/>
+    <col min="140" max="140" width="40.625" customWidth="1"/>
+    <col min="141" max="141" width="24.625" customWidth="1"/>
     <col min="142" max="142" width="13.5" customWidth="1"/>
-    <col min="143" max="143" width="24.1640625" customWidth="1"/>
+    <col min="143" max="143" width="24.125" customWidth="1"/>
     <col min="144" max="144" width="31" customWidth="1"/>
-    <col min="145" max="145" width="29.6640625" customWidth="1"/>
+    <col min="145" max="145" width="29.625" customWidth="1"/>
     <col min="146" max="146" width="30.5" customWidth="1"/>
     <col min="147" max="147" width="29" customWidth="1"/>
-    <col min="148" max="150" width="11.6640625" customWidth="1"/>
+    <col min="148" max="150" width="11.625" customWidth="1"/>
     <col min="151" max="151" width="10" customWidth="1"/>
-    <col min="152" max="152" width="9.6640625" customWidth="1"/>
+    <col min="152" max="152" width="9.625" customWidth="1"/>
     <col min="153" max="153" width="10" customWidth="1"/>
     <col min="154" max="154" width="10.5" customWidth="1"/>
     <col min="155" max="155" width="11.5" customWidth="1"/>
-    <col min="156" max="156" width="9.1640625" customWidth="1"/>
+    <col min="156" max="156" width="9.125" customWidth="1"/>
     <col min="157" max="157" width="10.5" customWidth="1"/>
-    <col min="158" max="158" width="9.1640625" customWidth="1"/>
-    <col min="159" max="159" width="11.1640625" customWidth="1"/>
-    <col min="160" max="160" width="39.1640625" customWidth="1"/>
-    <col min="161" max="161" width="19.1640625" customWidth="1"/>
-    <col min="162" max="162" width="20.1640625" customWidth="1"/>
+    <col min="158" max="158" width="9.125" customWidth="1"/>
+    <col min="159" max="159" width="11.125" customWidth="1"/>
+    <col min="160" max="160" width="39.125" customWidth="1"/>
+    <col min="161" max="161" width="19.125" customWidth="1"/>
+    <col min="162" max="162" width="20.125" customWidth="1"/>
     <col min="163" max="163" width="13" customWidth="1"/>
     <col min="164" max="164" width="29.5" customWidth="1"/>
-    <col min="165" max="165" width="30.1640625" customWidth="1"/>
-    <col min="166" max="166" width="30.6640625" customWidth="1"/>
+    <col min="165" max="165" width="30.125" customWidth="1"/>
+    <col min="166" max="166" width="30.625" customWidth="1"/>
     <col min="167" max="167" width="29" customWidth="1"/>
-    <col min="168" max="168" width="30.33203125" customWidth="1"/>
-    <col min="169" max="169" width="31.1640625" customWidth="1"/>
-    <col min="170" max="170" width="39.6640625" customWidth="1"/>
-    <col min="171" max="171" width="11.6640625" customWidth="1"/>
-    <col min="172" max="191" width="8.6640625" customWidth="1"/>
+    <col min="168" max="168" width="30.375" customWidth="1"/>
+    <col min="169" max="169" width="31.125" customWidth="1"/>
+    <col min="170" max="170" width="39.625" customWidth="1"/>
+    <col min="171" max="171" width="11.625" customWidth="1"/>
+    <col min="172" max="191" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="DZ1" s="2"/>
       <c r="EA1" s="2"/>
@@ -1935,12 +1935,12 @@
       <c r="GH1" s="3"/>
       <c r="GI1" s="3"/>
     </row>
-    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C2" s="2">
         <v>1.04</v>
@@ -2386,12 +2386,12 @@
       <c r="GH2" s="4"/>
       <c r="GI2" s="4"/>
     </row>
-    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C3" s="2">
         <v>30.7</v>
@@ -2837,12 +2837,12 @@
       <c r="GH3" s="4"/>
       <c r="GI3" s="4"/>
     </row>
-    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3288,12 +3288,12 @@
       <c r="GH4" s="4"/>
       <c r="GI4" s="4"/>
     </row>
-    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C5" s="2">
         <v>29.6</v>
@@ -3739,12 +3739,12 @@
       <c r="GH5" s="4"/>
       <c r="GI5" s="4"/>
     </row>
-    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C6" s="2">
         <v>30.5</v>
@@ -4190,12 +4190,12 @@
       <c r="GH6" s="4"/>
       <c r="GI6" s="4"/>
     </row>
-    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C7" s="2">
         <v>31.3</v>
@@ -4641,12 +4641,12 @@
       <c r="GH7" s="4"/>
       <c r="GI7" s="4"/>
     </row>
-    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C8" s="2">
         <v>30.2</v>
@@ -5092,12 +5092,12 @@
       <c r="GH8" s="4"/>
       <c r="GI8" s="4"/>
     </row>
-    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C9" s="2">
         <v>25.2</v>
@@ -5543,12 +5543,12 @@
       <c r="GH9" s="4"/>
       <c r="GI9" s="4"/>
     </row>
-    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C10" s="2">
         <v>29.5</v>
@@ -5994,12 +5994,12 @@
       <c r="GH10" s="4"/>
       <c r="GI10" s="4"/>
     </row>
-    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C11" s="2">
         <v>113.4</v>
@@ -6445,12 +6445,12 @@
       <c r="GH11" s="4"/>
       <c r="GI11" s="4"/>
     </row>
-    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C12" s="2">
         <v>28.4</v>
@@ -6896,12 +6896,12 @@
       <c r="GH12" s="4"/>
       <c r="GI12" s="4"/>
     </row>
-    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C13" s="2">
         <v>31.1</v>
@@ -7347,12 +7347,12 @@
       <c r="GH13" s="4"/>
       <c r="GI13" s="4"/>
     </row>
-    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C14" s="2">
         <v>31.3</v>
@@ -7798,12 +7798,12 @@
       <c r="GH14" s="4"/>
       <c r="GI14" s="4"/>
     </row>
-    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C15" s="2">
         <v>30.1</v>
@@ -8249,12 +8249,12 @@
       <c r="GH15" s="4"/>
       <c r="GI15" s="4"/>
     </row>
-    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C16" s="2">
         <v>29</v>
@@ -8700,12 +8700,12 @@
       <c r="GH16" s="4"/>
       <c r="GI16" s="4"/>
     </row>
-    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C17" s="2">
         <v>28.4</v>
@@ -9151,12 +9151,12 @@
       <c r="GH17" s="4"/>
       <c r="GI17" s="4"/>
     </row>
-    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C18" s="2">
         <v>30.7</v>
@@ -9602,12 +9602,12 @@
       <c r="GH18" s="4"/>
       <c r="GI18" s="4"/>
     </row>
-    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C19" s="2">
         <v>30.5</v>
@@ -10053,12 +10053,12 @@
       <c r="GH19" s="4"/>
       <c r="GI19" s="4"/>
     </row>
-    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C20" s="2">
         <v>30.7</v>
@@ -10504,12 +10504,12 @@
       <c r="GH20" s="4"/>
       <c r="GI20" s="4"/>
     </row>
-    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C21" s="2">
         <v>28.4</v>
@@ -10955,12 +10955,12 @@
       <c r="GH21" s="4"/>
       <c r="GI21" s="4"/>
     </row>
-    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C22" s="2">
         <v>28.4</v>
@@ -11406,12 +11406,12 @@
       <c r="GH22" s="4"/>
       <c r="GI22" s="4"/>
     </row>
-    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C23" s="2">
         <v>4.2</v>
@@ -11857,12 +11857,12 @@
       <c r="GH23" s="4"/>
       <c r="GI23" s="4"/>
     </row>
-    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C24" s="2">
         <v>28.4</v>
@@ -12308,12 +12308,12 @@
       <c r="GH24" s="4"/>
       <c r="GI24" s="4"/>
     </row>
-    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C25" s="2">
         <v>28.4</v>
@@ -12759,12 +12759,12 @@
       <c r="GH25" s="4"/>
       <c r="GI25" s="4"/>
     </row>
-    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C26" s="2">
         <v>28.4</v>
@@ -13210,12 +13210,12 @@
       <c r="GH26" s="4"/>
       <c r="GI26" s="4"/>
     </row>
-    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C27" s="2">
         <v>28.4</v>
@@ -13661,12 +13661,12 @@
       <c r="GH27" s="4"/>
       <c r="GI27" s="4"/>
     </row>
-    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C28" s="2">
         <v>35.1</v>
@@ -14112,12 +14112,12 @@
       <c r="GH28" s="4"/>
       <c r="GI28" s="4"/>
     </row>
-    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C29" s="2">
         <v>40.299999999999997</v>
@@ -14563,12 +14563,12 @@
       <c r="GH29" s="4"/>
       <c r="GI29" s="4"/>
     </row>
-    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C30" s="2">
         <v>45.8</v>
@@ -15014,12 +15014,12 @@
       <c r="GH30" s="4"/>
       <c r="GI30" s="4"/>
     </row>
-    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C31" s="2">
         <v>49.7</v>
@@ -15465,12 +15465,12 @@
       <c r="GH31" s="4"/>
       <c r="GI31" s="4"/>
     </row>
-    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C32" s="2">
         <v>4.5999999999999996</v>
@@ -15916,12 +15916,12 @@
       <c r="GH32" s="4"/>
       <c r="GI32" s="4"/>
     </row>
-    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -16367,12 +16367,12 @@
       <c r="GH33" s="4"/>
       <c r="GI33" s="4"/>
     </row>
-    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C34" s="2">
         <v>91.9</v>
@@ -16818,12 +16818,12 @@
       <c r="GH34" s="4"/>
       <c r="GI34" s="4"/>
     </row>
-    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C35" s="2">
         <v>28.4</v>
@@ -17269,12 +17269,12 @@
       <c r="GH35" s="4"/>
       <c r="GI35" s="4"/>
     </row>
-    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C36" s="2">
         <v>28.4</v>
@@ -17720,12 +17720,12 @@
       <c r="GH36" s="4"/>
       <c r="GI36" s="4"/>
     </row>
-    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C37" s="2">
         <v>30</v>
@@ -18171,12 +18171,12 @@
       <c r="GH37" s="4"/>
       <c r="GI37" s="4"/>
     </row>
-    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C38" s="2">
         <v>28.4</v>
@@ -18622,12 +18622,12 @@
       <c r="GH38" s="4"/>
       <c r="GI38" s="4"/>
     </row>
-    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C39" s="2">
         <v>28.4</v>
@@ -19073,12 +19073,12 @@
       <c r="GH39" s="4"/>
       <c r="GI39" s="4"/>
     </row>
-    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C40" s="2">
         <v>28.4</v>
@@ -19524,12 +19524,12 @@
       <c r="GH40" s="4"/>
       <c r="GI40" s="4"/>
     </row>
-    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C41" s="2">
         <v>28.4</v>
@@ -19975,12 +19975,12 @@
       <c r="GH41" s="4"/>
       <c r="GI41" s="4"/>
     </row>
-    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C42" s="2">
         <v>28.4</v>
@@ -20426,12 +20426,12 @@
       <c r="GH42" s="4"/>
       <c r="GI42" s="4"/>
     </row>
-    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C43" s="2">
         <v>28.4</v>
@@ -20877,12 +20877,12 @@
       <c r="GH43" s="4"/>
       <c r="GI43" s="4"/>
     </row>
-    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C44" s="2">
         <v>28.4</v>
@@ -21328,12 +21328,12 @@
       <c r="GH44" s="4"/>
       <c r="GI44" s="4"/>
     </row>
-    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C45" s="2">
         <v>28.4</v>
@@ -21779,12 +21779,12 @@
       <c r="GH45" s="4"/>
       <c r="GI45" s="4"/>
     </row>
-    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C46" s="2">
         <v>28.4</v>
@@ -22230,12 +22230,12 @@
       <c r="GH46" s="4"/>
       <c r="GI46" s="4"/>
     </row>
-    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C47" s="2">
         <v>28.4</v>
@@ -22681,12 +22681,12 @@
       <c r="GH47" s="4"/>
       <c r="GI47" s="4"/>
     </row>
-    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C48" s="2">
         <v>28.4</v>
@@ -23132,12 +23132,12 @@
       <c r="GH48" s="4"/>
       <c r="GI48" s="4"/>
     </row>
-    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C49" s="2">
         <v>28.4</v>
@@ -23583,12 +23583,12 @@
       <c r="GH49" s="4"/>
       <c r="GI49" s="4"/>
     </row>
-    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C50" s="2">
         <v>28.4</v>
@@ -24034,12 +24034,12 @@
       <c r="GH50" s="4"/>
       <c r="GI50" s="4"/>
     </row>
-    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C51" s="2">
         <v>28.4</v>
@@ -24485,12 +24485,12 @@
       <c r="GH51" s="4"/>
       <c r="GI51" s="4"/>
     </row>
-    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2">
         <v>28.4</v>
@@ -24936,12 +24936,12 @@
       <c r="GH52" s="4"/>
       <c r="GI52" s="4"/>
     </row>
-    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C53" s="2">
         <v>28.4</v>
@@ -25387,12 +25387,12 @@
       <c r="GH53" s="4"/>
       <c r="GI53" s="4"/>
     </row>
-    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C54" s="2">
         <v>28.4</v>
@@ -25838,12 +25838,12 @@
       <c r="GH54" s="4"/>
       <c r="GI54" s="4"/>
     </row>
-    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C55" s="2">
         <v>28.4</v>
@@ -26289,12 +26289,12 @@
       <c r="GH55" s="4"/>
       <c r="GI55" s="4"/>
     </row>
-    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C56" s="2">
         <v>28.4</v>
@@ -26740,12 +26740,12 @@
       <c r="GH56" s="4"/>
       <c r="GI56" s="4"/>
     </row>
-    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C57" s="2">
         <v>28.4</v>
@@ -27191,12 +27191,12 @@
       <c r="GH57" s="4"/>
       <c r="GI57" s="4"/>
     </row>
-    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C58" s="2">
         <v>28.4</v>
@@ -27642,12 +27642,12 @@
       <c r="GH58" s="4"/>
       <c r="GI58" s="4"/>
     </row>
-    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C59" s="2">
         <v>28.4</v>
@@ -28093,12 +28093,12 @@
       <c r="GH59" s="4"/>
       <c r="GI59" s="4"/>
     </row>
-    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C60" s="2">
         <v>28.4</v>
@@ -28544,12 +28544,12 @@
       <c r="GH60" s="2"/>
       <c r="GI60" s="2"/>
     </row>
-    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C61" s="2">
         <v>28.4</v>
@@ -28995,12 +28995,12 @@
       <c r="GH61" s="4"/>
       <c r="GI61" s="4"/>
     </row>
-    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C62" s="2">
         <v>28.4</v>
@@ -29446,12 +29446,12 @@
       <c r="GH62" s="4"/>
       <c r="GI62" s="4"/>
     </row>
-    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C63" s="2">
         <v>28.4</v>
@@ -29897,12 +29897,12 @@
       <c r="GH63" s="4"/>
       <c r="GI63" s="4"/>
     </row>
-    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C64" s="2">
         <v>28.4</v>
@@ -30348,12 +30348,12 @@
       <c r="GH64" s="4"/>
       <c r="GI64" s="4"/>
     </row>
-    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C65" s="2">
         <v>28.4</v>
@@ -30799,12 +30799,12 @@
       <c r="GH65" s="4"/>
       <c r="GI65" s="4"/>
     </row>
-    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C66" s="2">
         <v>28.4</v>
@@ -31250,12 +31250,12 @@
       <c r="GH66" s="4"/>
       <c r="GI66" s="4"/>
     </row>
-    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C67" s="2">
         <v>28.4</v>
@@ -31701,12 +31701,12 @@
       <c r="GH67" s="4"/>
       <c r="GI67" s="4"/>
     </row>
-    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C68" s="2">
         <v>28.4</v>
@@ -32152,12 +32152,12 @@
       <c r="GH68" s="4"/>
       <c r="GI68" s="4"/>
     </row>
-    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C69" s="2">
         <v>28.4</v>
@@ -32603,12 +32603,12 @@
       <c r="GH69" s="4"/>
       <c r="GI69" s="4"/>
     </row>
-    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C70" s="2">
         <v>28.4</v>
@@ -33054,12 +33054,12 @@
       <c r="GH70" s="4"/>
       <c r="GI70" s="4"/>
     </row>
-    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C71" s="2">
         <v>28.4</v>
@@ -33505,12 +33505,12 @@
       <c r="GH71" s="4"/>
       <c r="GI71" s="4"/>
     </row>
-    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C72" s="2">
         <v>28.4</v>
@@ -33956,12 +33956,12 @@
       <c r="GH72" s="4"/>
       <c r="GI72" s="4"/>
     </row>
-    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C73" s="2">
         <v>28.4</v>
@@ -34407,12 +34407,12 @@
       <c r="GH73" s="4"/>
       <c r="GI73" s="4"/>
     </row>
-    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C74" s="2">
         <v>28.4</v>
@@ -34858,12 +34858,12 @@
       <c r="GH74" s="4"/>
       <c r="GI74" s="4"/>
     </row>
-    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C75" s="2">
         <v>28.4</v>
@@ -35309,12 +35309,12 @@
       <c r="GH75" s="4"/>
       <c r="GI75" s="4"/>
     </row>
-    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C76" s="2">
         <v>28.4</v>
@@ -35760,12 +35760,12 @@
       <c r="GH76" s="4"/>
       <c r="GI76" s="4"/>
     </row>
-    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C77" s="2">
         <v>43.3</v>
@@ -36211,12 +36211,12 @@
       <c r="GH77" s="4"/>
       <c r="GI77" s="4"/>
     </row>
-    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C78" s="2">
         <v>28.4</v>
@@ -36662,12 +36662,12 @@
       <c r="GH78" s="4"/>
       <c r="GI78" s="4"/>
     </row>
-    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C79" s="2">
         <v>26.2</v>
@@ -37113,12 +37113,12 @@
       <c r="GH79" s="4"/>
       <c r="GI79" s="4"/>
     </row>
-    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C80" s="2">
         <v>59.4</v>
@@ -37564,12 +37564,12 @@
       <c r="GH80" s="4"/>
       <c r="GI80" s="4"/>
     </row>
-    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C81" s="2">
         <v>10.8</v>
@@ -38015,12 +38015,12 @@
       <c r="GH81" s="4"/>
       <c r="GI81" s="4"/>
     </row>
-    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C82" s="2">
         <v>6.8</v>
@@ -38466,12 +38466,12 @@
       <c r="GH82" s="4"/>
       <c r="GI82" s="4"/>
     </row>
-    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C83" s="2">
         <v>28.4</v>
@@ -38917,12 +38917,12 @@
       <c r="GH83" s="4"/>
       <c r="GI83" s="4"/>
     </row>
-    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C84" s="2">
         <v>4.7</v>
@@ -39368,12 +39368,12 @@
       <c r="GH84" s="4"/>
       <c r="GI84" s="4"/>
     </row>
-    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C85" s="6">
         <v>4.5</v>
@@ -39757,12 +39757,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C86" s="2">
         <v>31</v>

</xml_diff>

<commit_message>
Revert "Merge pull request #15 from mauro125/master"
This reverts commit 8ac9a8cd968828d76113318289b6e5b065941963, reversing
changes made to 464ae7f77c27b6671dc66fc1db31df8b2a526df2.
</commit_message>
<xml_diff>
--- a/src/main/resources/FFQRDatabase.xlsx
+++ b/src/main/resources/FFQRDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\BabyFeed\ffq-food-item-service\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcot/Documents/tmp/FIU/SP/Baby-feed/src/ffq-food-item-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C65B34B-3008-4FDA-9DB7-668971D25B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C6E35B-93F4-5342-BA6B-56BAA0EF8650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="2325" windowWidth="25380" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,16 @@
     <t>Total Grams</t>
   </si>
   <si>
+    <t>Energy (kcal)</t>
+  </si>
+  <si>
     <t>Total Fat (g)</t>
+  </si>
+  <si>
+    <t>Total Carbohydrate (g)</t>
+  </si>
+  <si>
+    <t>Total Protein (g)</t>
   </si>
   <si>
     <t>Animal Protein (g)</t>
@@ -42,6 +51,9 @@
   </si>
   <si>
     <t>Alcohol (g)</t>
+  </si>
+  <si>
+    <t>Cholesterol (mg)</t>
   </si>
   <si>
     <t>Total Saturated Fatty Acids (SFA) (g)</t>
@@ -128,7 +140,13 @@
     <t>Niacin (vitamin B3) (mg)</t>
   </si>
   <si>
+    <t>Pantothenic Acid (mg)</t>
+  </si>
+  <si>
     <t>Vitamin B-6 (pyridoxine, pyridoxyl, &amp; pyridoxamine) (mg)</t>
+  </si>
+  <si>
+    <t>Total Folate (mcg)</t>
   </si>
   <si>
     <t>Vitamin B-12 (cobalamin) (mcg)</t>
@@ -904,24 +922,6 @@
   <si>
     <t>pds</t>
   </si>
-  <si>
-    <t>Energy (kcal)</t>
-  </si>
-  <si>
-    <t>CHO (g)</t>
-  </si>
-  <si>
-    <t>Vitamin B9 (Folate) (mcg)</t>
-  </si>
-  <si>
-    <t>Cholesterol (mg)</t>
-  </si>
-  <si>
-    <t>Protein (g)</t>
-  </si>
-  <si>
-    <t>Vitamin B5 (Pantothenic acid) (mg)</t>
-  </si>
 </sst>
 </file>
 
@@ -1309,568 +1309,568 @@
   <dimension ref="A1:GI86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN1" sqref="AN1"/>
+      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="47.625" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
+    <col min="1" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.625" customWidth="1"/>
-    <col min="9" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="10" width="10.125" customWidth="1"/>
-    <col min="11" max="11" width="14.625" customWidth="1"/>
-    <col min="12" max="12" width="34.875" customWidth="1"/>
-    <col min="13" max="13" width="41.375" customWidth="1"/>
-    <col min="14" max="14" width="37.625" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="11.625" customWidth="1"/>
-    <col min="17" max="17" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" customWidth="1"/>
+    <col min="13" max="13" width="41.33203125" customWidth="1"/>
+    <col min="14" max="14" width="37.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="10.125" customWidth="1"/>
-    <col min="21" max="21" width="9.125" customWidth="1"/>
-    <col min="22" max="22" width="19.625" customWidth="1"/>
-    <col min="23" max="23" width="21.625" customWidth="1"/>
-    <col min="24" max="24" width="23.125" customWidth="1"/>
-    <col min="25" max="25" width="9.625" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" customWidth="1"/>
+    <col min="24" max="24" width="23.1640625" customWidth="1"/>
+    <col min="25" max="25" width="9.6640625" customWidth="1"/>
     <col min="26" max="26" width="45.5" customWidth="1"/>
-    <col min="27" max="27" width="29.125" customWidth="1"/>
-    <col min="28" max="28" width="12.125" customWidth="1"/>
-    <col min="29" max="29" width="14.625" customWidth="1"/>
+    <col min="27" max="27" width="29.1640625" customWidth="1"/>
+    <col min="28" max="28" width="12.1640625" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" customWidth="1"/>
     <col min="30" max="30" width="27.5" customWidth="1"/>
     <col min="31" max="31" width="32" customWidth="1"/>
-    <col min="32" max="32" width="16.625" customWidth="1"/>
-    <col min="33" max="34" width="17.125" customWidth="1"/>
-    <col min="35" max="35" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="14.625" customWidth="1"/>
-    <col min="39" max="39" width="26.375" customWidth="1"/>
-    <col min="40" max="40" width="25.625" customWidth="1"/>
-    <col min="41" max="41" width="33.375" customWidth="1"/>
-    <col min="42" max="42" width="16.375" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" customWidth="1"/>
+    <col min="33" max="34" width="17.1640625" customWidth="1"/>
+    <col min="35" max="35" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="14.6640625" customWidth="1"/>
+    <col min="39" max="39" width="26.33203125" customWidth="1"/>
+    <col min="40" max="40" width="25.6640625" customWidth="1"/>
+    <col min="41" max="41" width="33.33203125" customWidth="1"/>
+    <col min="42" max="42" width="16.33203125" customWidth="1"/>
     <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="11.625" customWidth="1"/>
+    <col min="44" max="44" width="11.6640625" customWidth="1"/>
     <col min="45" max="45" width="15.5" customWidth="1"/>
-    <col min="46" max="46" width="15.125" customWidth="1"/>
-    <col min="47" max="48" width="8.625" customWidth="1"/>
-    <col min="49" max="49" width="11.375" customWidth="1"/>
-    <col min="50" max="50" width="14.125" customWidth="1"/>
-    <col min="51" max="51" width="11.625" customWidth="1"/>
-    <col min="52" max="52" width="14.125" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" customWidth="1"/>
+    <col min="47" max="48" width="8.6640625" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" customWidth="1"/>
+    <col min="50" max="50" width="14.1640625" customWidth="1"/>
+    <col min="51" max="51" width="11.6640625" customWidth="1"/>
+    <col min="52" max="52" width="14.1640625" customWidth="1"/>
     <col min="53" max="53" width="22" customWidth="1"/>
-    <col min="54" max="54" width="22.125" customWidth="1"/>
+    <col min="54" max="54" width="22.1640625" customWidth="1"/>
     <col min="55" max="55" width="22.5" customWidth="1"/>
     <col min="56" max="56" width="22" customWidth="1"/>
-    <col min="57" max="57" width="21.625" customWidth="1"/>
-    <col min="58" max="59" width="23.625" customWidth="1"/>
-    <col min="60" max="60" width="24.375" customWidth="1"/>
+    <col min="57" max="57" width="21.6640625" customWidth="1"/>
+    <col min="58" max="59" width="23.6640625" customWidth="1"/>
+    <col min="60" max="60" width="24.33203125" customWidth="1"/>
     <col min="61" max="61" width="22.5" customWidth="1"/>
-    <col min="62" max="62" width="24.625" customWidth="1"/>
-    <col min="63" max="63" width="23.625" customWidth="1"/>
-    <col min="64" max="64" width="28.375" customWidth="1"/>
+    <col min="62" max="62" width="24.6640625" customWidth="1"/>
+    <col min="63" max="63" width="23.6640625" customWidth="1"/>
+    <col min="64" max="64" width="28.33203125" customWidth="1"/>
     <col min="65" max="65" width="28.5" customWidth="1"/>
-    <col min="66" max="66" width="22.625" customWidth="1"/>
-    <col min="67" max="67" width="26.125" customWidth="1"/>
+    <col min="66" max="66" width="22.6640625" customWidth="1"/>
+    <col min="67" max="67" width="26.1640625" customWidth="1"/>
     <col min="68" max="68" width="24" customWidth="1"/>
-    <col min="69" max="69" width="24.375" customWidth="1"/>
-    <col min="70" max="70" width="25.625" customWidth="1"/>
+    <col min="69" max="69" width="24.33203125" customWidth="1"/>
+    <col min="70" max="70" width="25.6640625" customWidth="1"/>
     <col min="71" max="71" width="26" customWidth="1"/>
-    <col min="72" max="72" width="28.375" customWidth="1"/>
-    <col min="73" max="73" width="38.625" customWidth="1"/>
-    <col min="74" max="74" width="39.625" customWidth="1"/>
-    <col min="75" max="75" width="38.625" customWidth="1"/>
-    <col min="76" max="76" width="13.625" customWidth="1"/>
-    <col min="77" max="77" width="12.375" customWidth="1"/>
-    <col min="78" max="78" width="12.125" customWidth="1"/>
-    <col min="79" max="79" width="10.125" customWidth="1"/>
-    <col min="80" max="80" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="13.625" customWidth="1"/>
-    <col min="82" max="82" width="9.625" customWidth="1"/>
-    <col min="83" max="83" width="15.625" customWidth="1"/>
-    <col min="84" max="84" width="10.625" customWidth="1"/>
-    <col min="85" max="85" width="8.625" customWidth="1"/>
-    <col min="86" max="86" width="10.625" customWidth="1"/>
-    <col min="87" max="87" width="11.125" customWidth="1"/>
-    <col min="88" max="88" width="10.125" customWidth="1"/>
+    <col min="72" max="72" width="28.33203125" customWidth="1"/>
+    <col min="73" max="73" width="38.6640625" customWidth="1"/>
+    <col min="74" max="74" width="39.6640625" customWidth="1"/>
+    <col min="75" max="75" width="38.6640625" customWidth="1"/>
+    <col min="76" max="76" width="13.6640625" customWidth="1"/>
+    <col min="77" max="77" width="12.33203125" customWidth="1"/>
+    <col min="78" max="78" width="12.1640625" customWidth="1"/>
+    <col min="79" max="79" width="10.1640625" customWidth="1"/>
+    <col min="80" max="80" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.6640625" customWidth="1"/>
+    <col min="82" max="82" width="9.6640625" customWidth="1"/>
+    <col min="83" max="83" width="15.6640625" customWidth="1"/>
+    <col min="84" max="84" width="10.6640625" customWidth="1"/>
+    <col min="85" max="85" width="8.6640625" customWidth="1"/>
+    <col min="86" max="86" width="10.6640625" customWidth="1"/>
+    <col min="87" max="87" width="11.1640625" customWidth="1"/>
+    <col min="88" max="88" width="10.1640625" customWidth="1"/>
     <col min="89" max="89" width="15" customWidth="1"/>
-    <col min="90" max="90" width="49.375" customWidth="1"/>
-    <col min="91" max="91" width="9.625" customWidth="1"/>
-    <col min="92" max="92" width="22.625" customWidth="1"/>
+    <col min="90" max="90" width="49.33203125" customWidth="1"/>
+    <col min="91" max="91" width="9.6640625" customWidth="1"/>
+    <col min="92" max="92" width="22.6640625" customWidth="1"/>
     <col min="93" max="93" width="9" customWidth="1"/>
-    <col min="94" max="94" width="14.625" customWidth="1"/>
-    <col min="95" max="95" width="13.625" customWidth="1"/>
-    <col min="96" max="96" width="12.125" customWidth="1"/>
+    <col min="94" max="94" width="14.6640625" customWidth="1"/>
+    <col min="95" max="95" width="13.6640625" customWidth="1"/>
+    <col min="96" max="96" width="12.1640625" customWidth="1"/>
     <col min="97" max="97" width="15" customWidth="1"/>
-    <col min="98" max="98" width="14.625" customWidth="1"/>
-    <col min="99" max="99" width="20.625" customWidth="1"/>
+    <col min="98" max="98" width="14.6640625" customWidth="1"/>
+    <col min="99" max="99" width="20.6640625" customWidth="1"/>
     <col min="100" max="100" width="19" customWidth="1"/>
-    <col min="101" max="101" width="6.625" customWidth="1"/>
+    <col min="101" max="101" width="6.6640625" customWidth="1"/>
     <col min="102" max="102" width="9" customWidth="1"/>
     <col min="103" max="103" width="17.5" customWidth="1"/>
-    <col min="104" max="104" width="26.625" customWidth="1"/>
-    <col min="105" max="105" width="21.375" customWidth="1"/>
+    <col min="104" max="104" width="26.6640625" customWidth="1"/>
+    <col min="105" max="105" width="21.33203125" customWidth="1"/>
     <col min="106" max="106" width="21.5" customWidth="1"/>
     <col min="107" max="107" width="18" customWidth="1"/>
     <col min="108" max="108" width="20" customWidth="1"/>
-    <col min="109" max="109" width="19.375" customWidth="1"/>
-    <col min="110" max="110" width="35.375" customWidth="1"/>
-    <col min="111" max="111" width="36.625" customWidth="1"/>
-    <col min="112" max="112" width="45.625" customWidth="1"/>
-    <col min="113" max="113" width="36.125" customWidth="1"/>
+    <col min="109" max="109" width="19.33203125" customWidth="1"/>
+    <col min="110" max="110" width="35.33203125" customWidth="1"/>
+    <col min="111" max="111" width="36.6640625" customWidth="1"/>
+    <col min="112" max="112" width="45.6640625" customWidth="1"/>
+    <col min="113" max="113" width="36.1640625" customWidth="1"/>
     <col min="114" max="114" width="39" customWidth="1"/>
     <col min="115" max="115" width="36.5" customWidth="1"/>
-    <col min="116" max="116" width="31.125" customWidth="1"/>
-    <col min="117" max="117" width="42.125" customWidth="1"/>
-    <col min="118" max="118" width="43.375" customWidth="1"/>
-    <col min="119" max="119" width="46.625" customWidth="1"/>
-    <col min="120" max="120" width="23.375" customWidth="1"/>
-    <col min="121" max="121" width="14.375" customWidth="1"/>
+    <col min="116" max="116" width="31.1640625" customWidth="1"/>
+    <col min="117" max="117" width="42.1640625" customWidth="1"/>
+    <col min="118" max="118" width="43.33203125" customWidth="1"/>
+    <col min="119" max="119" width="46.6640625" customWidth="1"/>
+    <col min="120" max="120" width="23.33203125" customWidth="1"/>
+    <col min="121" max="121" width="14.33203125" customWidth="1"/>
     <col min="122" max="122" width="29" customWidth="1"/>
-    <col min="123" max="123" width="30.125" customWidth="1"/>
+    <col min="123" max="123" width="30.1640625" customWidth="1"/>
     <col min="124" max="124" width="30" customWidth="1"/>
-    <col min="125" max="125" width="53.125" customWidth="1"/>
+    <col min="125" max="125" width="53.1640625" customWidth="1"/>
     <col min="126" max="126" width="10" customWidth="1"/>
-    <col min="127" max="127" width="21.375" customWidth="1"/>
-    <col min="128" max="128" width="14.125" customWidth="1"/>
+    <col min="127" max="127" width="21.33203125" customWidth="1"/>
+    <col min="128" max="128" width="14.1640625" customWidth="1"/>
     <col min="129" max="129" width="21.5" customWidth="1"/>
-    <col min="130" max="130" width="15.125" customWidth="1"/>
+    <col min="130" max="130" width="15.1640625" customWidth="1"/>
     <col min="131" max="131" width="12.5" customWidth="1"/>
-    <col min="132" max="132" width="28.125" customWidth="1"/>
-    <col min="133" max="133" width="29.625" customWidth="1"/>
+    <col min="132" max="132" width="28.1640625" customWidth="1"/>
+    <col min="133" max="133" width="29.6640625" customWidth="1"/>
     <col min="134" max="134" width="12.5" customWidth="1"/>
-    <col min="135" max="135" width="13.375" customWidth="1"/>
-    <col min="136" max="136" width="12.625" customWidth="1"/>
-    <col min="137" max="137" width="15.125" customWidth="1"/>
-    <col min="138" max="138" width="15.625" customWidth="1"/>
-    <col min="139" max="139" width="17.625" customWidth="1"/>
-    <col min="140" max="140" width="40.625" customWidth="1"/>
-    <col min="141" max="141" width="24.625" customWidth="1"/>
+    <col min="135" max="135" width="13.33203125" customWidth="1"/>
+    <col min="136" max="136" width="12.6640625" customWidth="1"/>
+    <col min="137" max="137" width="15.1640625" customWidth="1"/>
+    <col min="138" max="138" width="15.6640625" customWidth="1"/>
+    <col min="139" max="139" width="17.6640625" customWidth="1"/>
+    <col min="140" max="140" width="40.6640625" customWidth="1"/>
+    <col min="141" max="141" width="24.6640625" customWidth="1"/>
     <col min="142" max="142" width="13.5" customWidth="1"/>
-    <col min="143" max="143" width="24.125" customWidth="1"/>
+    <col min="143" max="143" width="24.1640625" customWidth="1"/>
     <col min="144" max="144" width="31" customWidth="1"/>
-    <col min="145" max="145" width="29.625" customWidth="1"/>
+    <col min="145" max="145" width="29.6640625" customWidth="1"/>
     <col min="146" max="146" width="30.5" customWidth="1"/>
     <col min="147" max="147" width="29" customWidth="1"/>
-    <col min="148" max="150" width="11.625" customWidth="1"/>
+    <col min="148" max="150" width="11.6640625" customWidth="1"/>
     <col min="151" max="151" width="10" customWidth="1"/>
-    <col min="152" max="152" width="9.625" customWidth="1"/>
+    <col min="152" max="152" width="9.6640625" customWidth="1"/>
     <col min="153" max="153" width="10" customWidth="1"/>
     <col min="154" max="154" width="10.5" customWidth="1"/>
     <col min="155" max="155" width="11.5" customWidth="1"/>
-    <col min="156" max="156" width="9.125" customWidth="1"/>
+    <col min="156" max="156" width="9.1640625" customWidth="1"/>
     <col min="157" max="157" width="10.5" customWidth="1"/>
-    <col min="158" max="158" width="9.125" customWidth="1"/>
-    <col min="159" max="159" width="11.125" customWidth="1"/>
-    <col min="160" max="160" width="39.125" customWidth="1"/>
-    <col min="161" max="161" width="19.125" customWidth="1"/>
-    <col min="162" max="162" width="20.125" customWidth="1"/>
+    <col min="158" max="158" width="9.1640625" customWidth="1"/>
+    <col min="159" max="159" width="11.1640625" customWidth="1"/>
+    <col min="160" max="160" width="39.1640625" customWidth="1"/>
+    <col min="161" max="161" width="19.1640625" customWidth="1"/>
+    <col min="162" max="162" width="20.1640625" customWidth="1"/>
     <col min="163" max="163" width="13" customWidth="1"/>
     <col min="164" max="164" width="29.5" customWidth="1"/>
-    <col min="165" max="165" width="30.125" customWidth="1"/>
-    <col min="166" max="166" width="30.625" customWidth="1"/>
+    <col min="165" max="165" width="30.1640625" customWidth="1"/>
+    <col min="166" max="166" width="30.6640625" customWidth="1"/>
     <col min="167" max="167" width="29" customWidth="1"/>
-    <col min="168" max="168" width="30.375" customWidth="1"/>
-    <col min="169" max="169" width="31.125" customWidth="1"/>
-    <col min="170" max="170" width="39.625" customWidth="1"/>
-    <col min="171" max="171" width="11.625" customWidth="1"/>
-    <col min="172" max="191" width="8.625" customWidth="1"/>
+    <col min="168" max="168" width="30.33203125" customWidth="1"/>
+    <col min="169" max="169" width="31.1640625" customWidth="1"/>
+    <col min="170" max="170" width="39.6640625" customWidth="1"/>
+    <col min="171" max="171" width="11.6640625" customWidth="1"/>
+    <col min="172" max="191" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>293</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>297</v>
+        <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>296</v>
+        <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>298</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>295</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="BO1" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="BS1" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="BT1" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="BU1" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="BX1" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="BY1" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="BZ1" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="CA1" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="CB1" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="CC1" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="CE1" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="CF1" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="CG1" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="CH1" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="CI1" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="CJ1" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="CK1" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="CL1" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="CM1" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="CN1" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="CO1" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="CP1" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="CQ1" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="CR1" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="CS1" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="CT1" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="CU1" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="CV1" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="CW1" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="CX1" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="CY1" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="CZ1" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="DA1" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="DB1" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="DC1" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="DE1" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="DF1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="DG1" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="DH1" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="DI1" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="DJ1" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="DK1" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="DL1" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="DM1" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="DN1" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="DO1" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="DP1" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="DQ1" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="DR1" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="DS1" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="DT1" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="DU1" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="DV1" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="DW1" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="DX1" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="DY1" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="DZ1" s="2"/>
       <c r="EA1" s="2"/>
@@ -1935,12 +1935,12 @@
       <c r="GH1" s="3"/>
       <c r="GI1" s="3"/>
     </row>
-    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C2" s="2">
         <v>1.04</v>
@@ -2386,12 +2386,12 @@
       <c r="GH2" s="4"/>
       <c r="GI2" s="4"/>
     </row>
-    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C3" s="2">
         <v>30.7</v>
@@ -2837,12 +2837,12 @@
       <c r="GH3" s="4"/>
       <c r="GI3" s="4"/>
     </row>
-    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3288,12 +3288,12 @@
       <c r="GH4" s="4"/>
       <c r="GI4" s="4"/>
     </row>
-    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C5" s="2">
         <v>29.6</v>
@@ -3739,12 +3739,12 @@
       <c r="GH5" s="4"/>
       <c r="GI5" s="4"/>
     </row>
-    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C6" s="2">
         <v>30.5</v>
@@ -4190,12 +4190,12 @@
       <c r="GH6" s="4"/>
       <c r="GI6" s="4"/>
     </row>
-    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C7" s="2">
         <v>31.3</v>
@@ -4641,12 +4641,12 @@
       <c r="GH7" s="4"/>
       <c r="GI7" s="4"/>
     </row>
-    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C8" s="2">
         <v>30.2</v>
@@ -5092,12 +5092,12 @@
       <c r="GH8" s="4"/>
       <c r="GI8" s="4"/>
     </row>
-    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C9" s="2">
         <v>25.2</v>
@@ -5543,12 +5543,12 @@
       <c r="GH9" s="4"/>
       <c r="GI9" s="4"/>
     </row>
-    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C10" s="2">
         <v>29.5</v>
@@ -5994,12 +5994,12 @@
       <c r="GH10" s="4"/>
       <c r="GI10" s="4"/>
     </row>
-    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2">
         <v>113.4</v>
@@ -6445,12 +6445,12 @@
       <c r="GH11" s="4"/>
       <c r="GI11" s="4"/>
     </row>
-    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C12" s="2">
         <v>28.4</v>
@@ -6896,12 +6896,12 @@
       <c r="GH12" s="4"/>
       <c r="GI12" s="4"/>
     </row>
-    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C13" s="2">
         <v>31.1</v>
@@ -7347,12 +7347,12 @@
       <c r="GH13" s="4"/>
       <c r="GI13" s="4"/>
     </row>
-    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C14" s="2">
         <v>31.3</v>
@@ -7798,12 +7798,12 @@
       <c r="GH14" s="4"/>
       <c r="GI14" s="4"/>
     </row>
-    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C15" s="2">
         <v>30.1</v>
@@ -8249,12 +8249,12 @@
       <c r="GH15" s="4"/>
       <c r="GI15" s="4"/>
     </row>
-    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C16" s="2">
         <v>29</v>
@@ -8700,12 +8700,12 @@
       <c r="GH16" s="4"/>
       <c r="GI16" s="4"/>
     </row>
-    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C17" s="2">
         <v>28.4</v>
@@ -9151,12 +9151,12 @@
       <c r="GH17" s="4"/>
       <c r="GI17" s="4"/>
     </row>
-    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C18" s="2">
         <v>30.7</v>
@@ -9602,12 +9602,12 @@
       <c r="GH18" s="4"/>
       <c r="GI18" s="4"/>
     </row>
-    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C19" s="2">
         <v>30.5</v>
@@ -10053,12 +10053,12 @@
       <c r="GH19" s="4"/>
       <c r="GI19" s="4"/>
     </row>
-    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2">
         <v>30.7</v>
@@ -10504,12 +10504,12 @@
       <c r="GH20" s="4"/>
       <c r="GI20" s="4"/>
     </row>
-    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C21" s="2">
         <v>28.4</v>
@@ -10955,12 +10955,12 @@
       <c r="GH21" s="4"/>
       <c r="GI21" s="4"/>
     </row>
-    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C22" s="2">
         <v>28.4</v>
@@ -11406,12 +11406,12 @@
       <c r="GH22" s="4"/>
       <c r="GI22" s="4"/>
     </row>
-    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C23" s="2">
         <v>4.2</v>
@@ -11857,12 +11857,12 @@
       <c r="GH23" s="4"/>
       <c r="GI23" s="4"/>
     </row>
-    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C24" s="2">
         <v>28.4</v>
@@ -12308,12 +12308,12 @@
       <c r="GH24" s="4"/>
       <c r="GI24" s="4"/>
     </row>
-    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C25" s="2">
         <v>28.4</v>
@@ -12759,12 +12759,12 @@
       <c r="GH25" s="4"/>
       <c r="GI25" s="4"/>
     </row>
-    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C26" s="2">
         <v>28.4</v>
@@ -13210,12 +13210,12 @@
       <c r="GH26" s="4"/>
       <c r="GI26" s="4"/>
     </row>
-    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C27" s="2">
         <v>28.4</v>
@@ -13661,12 +13661,12 @@
       <c r="GH27" s="4"/>
       <c r="GI27" s="4"/>
     </row>
-    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C28" s="2">
         <v>35.1</v>
@@ -14112,12 +14112,12 @@
       <c r="GH28" s="4"/>
       <c r="GI28" s="4"/>
     </row>
-    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C29" s="2">
         <v>40.299999999999997</v>
@@ -14563,12 +14563,12 @@
       <c r="GH29" s="4"/>
       <c r="GI29" s="4"/>
     </row>
-    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C30" s="2">
         <v>45.8</v>
@@ -15014,12 +15014,12 @@
       <c r="GH30" s="4"/>
       <c r="GI30" s="4"/>
     </row>
-    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C31" s="2">
         <v>49.7</v>
@@ -15465,12 +15465,12 @@
       <c r="GH31" s="4"/>
       <c r="GI31" s="4"/>
     </row>
-    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C32" s="2">
         <v>4.5999999999999996</v>
@@ -15916,12 +15916,12 @@
       <c r="GH32" s="4"/>
       <c r="GI32" s="4"/>
     </row>
-    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -16367,12 +16367,12 @@
       <c r="GH33" s="4"/>
       <c r="GI33" s="4"/>
     </row>
-    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C34" s="2">
         <v>91.9</v>
@@ -16818,12 +16818,12 @@
       <c r="GH34" s="4"/>
       <c r="GI34" s="4"/>
     </row>
-    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C35" s="2">
         <v>28.4</v>
@@ -17269,12 +17269,12 @@
       <c r="GH35" s="4"/>
       <c r="GI35" s="4"/>
     </row>
-    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C36" s="2">
         <v>28.4</v>
@@ -17720,12 +17720,12 @@
       <c r="GH36" s="4"/>
       <c r="GI36" s="4"/>
     </row>
-    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C37" s="2">
         <v>30</v>
@@ -18171,12 +18171,12 @@
       <c r="GH37" s="4"/>
       <c r="GI37" s="4"/>
     </row>
-    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C38" s="2">
         <v>28.4</v>
@@ -18622,12 +18622,12 @@
       <c r="GH38" s="4"/>
       <c r="GI38" s="4"/>
     </row>
-    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C39" s="2">
         <v>28.4</v>
@@ -19073,12 +19073,12 @@
       <c r="GH39" s="4"/>
       <c r="GI39" s="4"/>
     </row>
-    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C40" s="2">
         <v>28.4</v>
@@ -19524,12 +19524,12 @@
       <c r="GH40" s="4"/>
       <c r="GI40" s="4"/>
     </row>
-    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C41" s="2">
         <v>28.4</v>
@@ -19975,12 +19975,12 @@
       <c r="GH41" s="4"/>
       <c r="GI41" s="4"/>
     </row>
-    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C42" s="2">
         <v>28.4</v>
@@ -20426,12 +20426,12 @@
       <c r="GH42" s="4"/>
       <c r="GI42" s="4"/>
     </row>
-    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C43" s="2">
         <v>28.4</v>
@@ -20877,12 +20877,12 @@
       <c r="GH43" s="4"/>
       <c r="GI43" s="4"/>
     </row>
-    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C44" s="2">
         <v>28.4</v>
@@ -21328,12 +21328,12 @@
       <c r="GH44" s="4"/>
       <c r="GI44" s="4"/>
     </row>
-    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C45" s="2">
         <v>28.4</v>
@@ -21779,12 +21779,12 @@
       <c r="GH45" s="4"/>
       <c r="GI45" s="4"/>
     </row>
-    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C46" s="2">
         <v>28.4</v>
@@ -22230,12 +22230,12 @@
       <c r="GH46" s="4"/>
       <c r="GI46" s="4"/>
     </row>
-    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C47" s="2">
         <v>28.4</v>
@@ -22681,12 +22681,12 @@
       <c r="GH47" s="4"/>
       <c r="GI47" s="4"/>
     </row>
-    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C48" s="2">
         <v>28.4</v>
@@ -23132,12 +23132,12 @@
       <c r="GH48" s="4"/>
       <c r="GI48" s="4"/>
     </row>
-    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C49" s="2">
         <v>28.4</v>
@@ -23583,12 +23583,12 @@
       <c r="GH49" s="4"/>
       <c r="GI49" s="4"/>
     </row>
-    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C50" s="2">
         <v>28.4</v>
@@ -24034,12 +24034,12 @@
       <c r="GH50" s="4"/>
       <c r="GI50" s="4"/>
     </row>
-    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C51" s="2">
         <v>28.4</v>
@@ -24485,12 +24485,12 @@
       <c r="GH51" s="4"/>
       <c r="GI51" s="4"/>
     </row>
-    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C52" s="2">
         <v>28.4</v>
@@ -24936,12 +24936,12 @@
       <c r="GH52" s="4"/>
       <c r="GI52" s="4"/>
     </row>
-    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C53" s="2">
         <v>28.4</v>
@@ -25387,12 +25387,12 @@
       <c r="GH53" s="4"/>
       <c r="GI53" s="4"/>
     </row>
-    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C54" s="2">
         <v>28.4</v>
@@ -25838,12 +25838,12 @@
       <c r="GH54" s="4"/>
       <c r="GI54" s="4"/>
     </row>
-    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C55" s="2">
         <v>28.4</v>
@@ -26289,12 +26289,12 @@
       <c r="GH55" s="4"/>
       <c r="GI55" s="4"/>
     </row>
-    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C56" s="2">
         <v>28.4</v>
@@ -26740,12 +26740,12 @@
       <c r="GH56" s="4"/>
       <c r="GI56" s="4"/>
     </row>
-    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C57" s="2">
         <v>28.4</v>
@@ -27191,12 +27191,12 @@
       <c r="GH57" s="4"/>
       <c r="GI57" s="4"/>
     </row>
-    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C58" s="2">
         <v>28.4</v>
@@ -27642,12 +27642,12 @@
       <c r="GH58" s="4"/>
       <c r="GI58" s="4"/>
     </row>
-    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C59" s="2">
         <v>28.4</v>
@@ -28093,12 +28093,12 @@
       <c r="GH59" s="4"/>
       <c r="GI59" s="4"/>
     </row>
-    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C60" s="2">
         <v>28.4</v>
@@ -28544,12 +28544,12 @@
       <c r="GH60" s="2"/>
       <c r="GI60" s="2"/>
     </row>
-    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C61" s="2">
         <v>28.4</v>
@@ -28995,12 +28995,12 @@
       <c r="GH61" s="4"/>
       <c r="GI61" s="4"/>
     </row>
-    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C62" s="2">
         <v>28.4</v>
@@ -29446,12 +29446,12 @@
       <c r="GH62" s="4"/>
       <c r="GI62" s="4"/>
     </row>
-    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C63" s="2">
         <v>28.4</v>
@@ -29897,12 +29897,12 @@
       <c r="GH63" s="4"/>
       <c r="GI63" s="4"/>
     </row>
-    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C64" s="2">
         <v>28.4</v>
@@ -30348,12 +30348,12 @@
       <c r="GH64" s="4"/>
       <c r="GI64" s="4"/>
     </row>
-    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C65" s="2">
         <v>28.4</v>
@@ -30799,12 +30799,12 @@
       <c r="GH65" s="4"/>
       <c r="GI65" s="4"/>
     </row>
-    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C66" s="2">
         <v>28.4</v>
@@ -31250,12 +31250,12 @@
       <c r="GH66" s="4"/>
       <c r="GI66" s="4"/>
     </row>
-    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C67" s="2">
         <v>28.4</v>
@@ -31701,12 +31701,12 @@
       <c r="GH67" s="4"/>
       <c r="GI67" s="4"/>
     </row>
-    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C68" s="2">
         <v>28.4</v>
@@ -32152,12 +32152,12 @@
       <c r="GH68" s="4"/>
       <c r="GI68" s="4"/>
     </row>
-    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C69" s="2">
         <v>28.4</v>
@@ -32603,12 +32603,12 @@
       <c r="GH69" s="4"/>
       <c r="GI69" s="4"/>
     </row>
-    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C70" s="2">
         <v>28.4</v>
@@ -33054,12 +33054,12 @@
       <c r="GH70" s="4"/>
       <c r="GI70" s="4"/>
     </row>
-    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C71" s="2">
         <v>28.4</v>
@@ -33505,12 +33505,12 @@
       <c r="GH71" s="4"/>
       <c r="GI71" s="4"/>
     </row>
-    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C72" s="2">
         <v>28.4</v>
@@ -33956,12 +33956,12 @@
       <c r="GH72" s="4"/>
       <c r="GI72" s="4"/>
     </row>
-    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C73" s="2">
         <v>28.4</v>
@@ -34407,12 +34407,12 @@
       <c r="GH73" s="4"/>
       <c r="GI73" s="4"/>
     </row>
-    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C74" s="2">
         <v>28.4</v>
@@ -34858,12 +34858,12 @@
       <c r="GH74" s="4"/>
       <c r="GI74" s="4"/>
     </row>
-    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C75" s="2">
         <v>28.4</v>
@@ -35309,12 +35309,12 @@
       <c r="GH75" s="4"/>
       <c r="GI75" s="4"/>
     </row>
-    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C76" s="2">
         <v>28.4</v>
@@ -35760,12 +35760,12 @@
       <c r="GH76" s="4"/>
       <c r="GI76" s="4"/>
     </row>
-    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C77" s="2">
         <v>43.3</v>
@@ -36211,12 +36211,12 @@
       <c r="GH77" s="4"/>
       <c r="GI77" s="4"/>
     </row>
-    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C78" s="2">
         <v>28.4</v>
@@ -36662,12 +36662,12 @@
       <c r="GH78" s="4"/>
       <c r="GI78" s="4"/>
     </row>
-    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C79" s="2">
         <v>26.2</v>
@@ -37113,12 +37113,12 @@
       <c r="GH79" s="4"/>
       <c r="GI79" s="4"/>
     </row>
-    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C80" s="2">
         <v>59.4</v>
@@ -37564,12 +37564,12 @@
       <c r="GH80" s="4"/>
       <c r="GI80" s="4"/>
     </row>
-    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C81" s="2">
         <v>10.8</v>
@@ -38015,12 +38015,12 @@
       <c r="GH81" s="4"/>
       <c r="GI81" s="4"/>
     </row>
-    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C82" s="2">
         <v>6.8</v>
@@ -38466,12 +38466,12 @@
       <c r="GH82" s="4"/>
       <c r="GI82" s="4"/>
     </row>
-    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C83" s="2">
         <v>28.4</v>
@@ -38917,12 +38917,12 @@
       <c r="GH83" s="4"/>
       <c r="GI83" s="4"/>
     </row>
-    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C84" s="2">
         <v>4.7</v>
@@ -39368,12 +39368,12 @@
       <c r="GH84" s="4"/>
       <c r="GI84" s="4"/>
     </row>
-    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C85" s="6">
         <v>4.5</v>
@@ -39757,12 +39757,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C86" s="2">
         <v>31</v>

</xml_diff>

<commit_message>
Update total carbs to CHO in the excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/FFQRDatabase.xlsx
+++ b/src/main/resources/FFQRDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcot/Documents/tmp/FIU/SP/Baby-feed/src/ffq-food-item-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afesyun/src/fiu/ffq-food-item-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C6E35B-93F4-5342-BA6B-56BAA0EF8650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B827D7DE-C5AD-A04F-BCB6-5DA865A01A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Total Fat (g)</t>
-  </si>
-  <si>
-    <t>Total Carbohydrate (g)</t>
   </si>
   <si>
     <t>Total Protein (g)</t>
@@ -922,6 +919,9 @@
   <si>
     <t>pds</t>
   </si>
+  <si>
+    <t>CHO (g)</t>
+  </si>
 </sst>
 </file>
 
@@ -1309,10 +1309,10 @@
   <dimension ref="A1:GI86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1501,376 +1501,376 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="DZ1" s="2"/>
       <c r="EA1" s="2"/>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="2">
         <v>1.04</v>
@@ -2388,10 +2388,10 @@
     </row>
     <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="2">
         <v>30.7</v>
@@ -2839,10 +2839,10 @@
     </row>
     <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3290,10 +3290,10 @@
     </row>
     <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="2">
         <v>29.6</v>
@@ -3741,10 +3741,10 @@
     </row>
     <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="2">
         <v>30.5</v>
@@ -4192,10 +4192,10 @@
     </row>
     <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="2">
         <v>31.3</v>
@@ -4643,10 +4643,10 @@
     </row>
     <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="2">
         <v>30.2</v>
@@ -5094,10 +5094,10 @@
     </row>
     <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="2">
         <v>25.2</v>
@@ -5545,10 +5545,10 @@
     </row>
     <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" s="2">
         <v>29.5</v>
@@ -5996,10 +5996,10 @@
     </row>
     <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C11" s="2">
         <v>113.4</v>
@@ -6447,10 +6447,10 @@
     </row>
     <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="2">
         <v>28.4</v>
@@ -6898,10 +6898,10 @@
     </row>
     <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="2">
         <v>31.1</v>
@@ -7349,10 +7349,10 @@
     </row>
     <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C14" s="2">
         <v>31.3</v>
@@ -7800,10 +7800,10 @@
     </row>
     <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="2">
         <v>30.1</v>
@@ -8251,10 +8251,10 @@
     </row>
     <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C16" s="2">
         <v>29</v>
@@ -8702,10 +8702,10 @@
     </row>
     <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C17" s="2">
         <v>28.4</v>
@@ -9153,10 +9153,10 @@
     </row>
     <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18" s="2">
         <v>30.7</v>
@@ -9604,10 +9604,10 @@
     </row>
     <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C19" s="2">
         <v>30.5</v>
@@ -10055,10 +10055,10 @@
     </row>
     <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C20" s="2">
         <v>30.7</v>
@@ -10506,10 +10506,10 @@
     </row>
     <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C21" s="2">
         <v>28.4</v>
@@ -10957,10 +10957,10 @@
     </row>
     <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C22" s="2">
         <v>28.4</v>
@@ -11408,10 +11408,10 @@
     </row>
     <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="2">
         <v>4.2</v>
@@ -11859,10 +11859,10 @@
     </row>
     <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C24" s="2">
         <v>28.4</v>
@@ -12310,10 +12310,10 @@
     </row>
     <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2">
         <v>28.4</v>
@@ -12761,10 +12761,10 @@
     </row>
     <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C26" s="2">
         <v>28.4</v>
@@ -13212,10 +13212,10 @@
     </row>
     <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C27" s="2">
         <v>28.4</v>
@@ -13663,10 +13663,10 @@
     </row>
     <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" s="2">
         <v>35.1</v>
@@ -14114,10 +14114,10 @@
     </row>
     <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" s="2">
         <v>40.299999999999997</v>
@@ -14565,10 +14565,10 @@
     </row>
     <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C30" s="2">
         <v>45.8</v>
@@ -15016,10 +15016,10 @@
     </row>
     <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C31" s="2">
         <v>49.7</v>
@@ -15467,10 +15467,10 @@
     </row>
     <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" s="2">
         <v>4.5999999999999996</v>
@@ -15918,10 +15918,10 @@
     </row>
     <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -16369,10 +16369,10 @@
     </row>
     <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C34" s="2">
         <v>91.9</v>
@@ -16820,10 +16820,10 @@
     </row>
     <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C35" s="2">
         <v>28.4</v>
@@ -17271,10 +17271,10 @@
     </row>
     <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C36" s="2">
         <v>28.4</v>
@@ -17722,10 +17722,10 @@
     </row>
     <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C37" s="2">
         <v>30</v>
@@ -18173,10 +18173,10 @@
     </row>
     <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C38" s="2">
         <v>28.4</v>
@@ -18624,10 +18624,10 @@
     </row>
     <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C39" s="2">
         <v>28.4</v>
@@ -19075,10 +19075,10 @@
     </row>
     <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C40" s="2">
         <v>28.4</v>
@@ -19526,10 +19526,10 @@
     </row>
     <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C41" s="2">
         <v>28.4</v>
@@ -19977,10 +19977,10 @@
     </row>
     <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C42" s="2">
         <v>28.4</v>
@@ -20428,10 +20428,10 @@
     </row>
     <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C43" s="2">
         <v>28.4</v>
@@ -20879,10 +20879,10 @@
     </row>
     <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C44" s="2">
         <v>28.4</v>
@@ -21330,10 +21330,10 @@
     </row>
     <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C45" s="2">
         <v>28.4</v>
@@ -21781,10 +21781,10 @@
     </row>
     <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C46" s="2">
         <v>28.4</v>
@@ -22232,10 +22232,10 @@
     </row>
     <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C47" s="2">
         <v>28.4</v>
@@ -22683,10 +22683,10 @@
     </row>
     <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C48" s="2">
         <v>28.4</v>
@@ -23134,10 +23134,10 @@
     </row>
     <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C49" s="2">
         <v>28.4</v>
@@ -23585,10 +23585,10 @@
     </row>
     <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C50" s="2">
         <v>28.4</v>
@@ -24036,10 +24036,10 @@
     </row>
     <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C51" s="2">
         <v>28.4</v>
@@ -24487,10 +24487,10 @@
     </row>
     <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C52" s="2">
         <v>28.4</v>
@@ -24938,10 +24938,10 @@
     </row>
     <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C53" s="2">
         <v>28.4</v>
@@ -25389,10 +25389,10 @@
     </row>
     <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C54" s="2">
         <v>28.4</v>
@@ -25840,10 +25840,10 @@
     </row>
     <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C55" s="2">
         <v>28.4</v>
@@ -26291,10 +26291,10 @@
     </row>
     <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C56" s="2">
         <v>28.4</v>
@@ -26742,10 +26742,10 @@
     </row>
     <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C57" s="2">
         <v>28.4</v>
@@ -27193,10 +27193,10 @@
     </row>
     <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C58" s="2">
         <v>28.4</v>
@@ -27644,10 +27644,10 @@
     </row>
     <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C59" s="2">
         <v>28.4</v>
@@ -28095,10 +28095,10 @@
     </row>
     <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C60" s="2">
         <v>28.4</v>
@@ -28546,10 +28546,10 @@
     </row>
     <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C61" s="2">
         <v>28.4</v>
@@ -28997,10 +28997,10 @@
     </row>
     <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C62" s="2">
         <v>28.4</v>
@@ -29448,10 +29448,10 @@
     </row>
     <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C63" s="2">
         <v>28.4</v>
@@ -29899,10 +29899,10 @@
     </row>
     <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C64" s="2">
         <v>28.4</v>
@@ -30350,10 +30350,10 @@
     </row>
     <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C65" s="2">
         <v>28.4</v>
@@ -30801,10 +30801,10 @@
     </row>
     <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C66" s="2">
         <v>28.4</v>
@@ -31252,10 +31252,10 @@
     </row>
     <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C67" s="2">
         <v>28.4</v>
@@ -31703,10 +31703,10 @@
     </row>
     <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C68" s="2">
         <v>28.4</v>
@@ -32154,10 +32154,10 @@
     </row>
     <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C69" s="2">
         <v>28.4</v>
@@ -32605,10 +32605,10 @@
     </row>
     <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C70" s="2">
         <v>28.4</v>
@@ -33056,10 +33056,10 @@
     </row>
     <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C71" s="2">
         <v>28.4</v>
@@ -33507,10 +33507,10 @@
     </row>
     <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C72" s="2">
         <v>28.4</v>
@@ -33958,10 +33958,10 @@
     </row>
     <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C73" s="2">
         <v>28.4</v>
@@ -34409,10 +34409,10 @@
     </row>
     <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C74" s="2">
         <v>28.4</v>
@@ -34860,10 +34860,10 @@
     </row>
     <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C75" s="2">
         <v>28.4</v>
@@ -35311,10 +35311,10 @@
     </row>
     <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C76" s="2">
         <v>28.4</v>
@@ -35762,10 +35762,10 @@
     </row>
     <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C77" s="2">
         <v>43.3</v>
@@ -36213,10 +36213,10 @@
     </row>
     <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C78" s="2">
         <v>28.4</v>
@@ -36664,10 +36664,10 @@
     </row>
     <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C79" s="2">
         <v>26.2</v>
@@ -37115,10 +37115,10 @@
     </row>
     <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C80" s="2">
         <v>59.4</v>
@@ -37566,10 +37566,10 @@
     </row>
     <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C81" s="2">
         <v>10.8</v>
@@ -38017,10 +38017,10 @@
     </row>
     <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C82" s="2">
         <v>6.8</v>
@@ -38468,10 +38468,10 @@
     </row>
     <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C83" s="2">
         <v>28.4</v>
@@ -38919,10 +38919,10 @@
     </row>
     <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C84" s="2">
         <v>4.7</v>
@@ -39370,10 +39370,10 @@
     </row>
     <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C85" s="6">
         <v>4.5</v>
@@ -39759,10 +39759,10 @@
     </row>
     <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="C86" s="2">
         <v>31</v>

</xml_diff>

<commit_message>
updating nutrient results and breakdown
</commit_message>
<xml_diff>
--- a/src/main/resources/FFQRDatabase.xlsx
+++ b/src/main/resources/FFQRDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afesyun/src/fiu/ffq-food-item-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\BabyFeed\ffq-food-item-service\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B827D7DE-C5AD-A04F-BCB6-5DA865A01A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1087D134-BCE4-4131-80E6-3E60D01BD50F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>Energy (kcal)</t>
-  </si>
-  <si>
-    <t>Total Fat (g)</t>
-  </si>
-  <si>
-    <t>Total Protein (g)</t>
   </si>
   <si>
     <t>Animal Protein (g)</t>
@@ -104,13 +98,7 @@
     <t>Retinol (mcg)</t>
   </si>
   <si>
-    <t>Vitamin D (calciferol) (mcg)</t>
-  </si>
-  <si>
     <t>Total Alpha-Tocopherol Equivalents (mg)</t>
-  </si>
-  <si>
-    <t>Vitamin E (Total Alpha-Tocopherol) (mg)</t>
   </si>
   <si>
     <t>Beta-Tocopherol (mg)</t>
@@ -120,33 +108,6 @@
   </si>
   <si>
     <t>Delta-Tocopherol (mg)</t>
-  </si>
-  <si>
-    <t>Vitamin K (phylloquinone) (mcg)</t>
-  </si>
-  <si>
-    <t>Vitamin C (ascorbic acid) (mg)</t>
-  </si>
-  <si>
-    <t>Thiamin (vitamin B1) (mg)</t>
-  </si>
-  <si>
-    <t>Riboflavin (vitamin B2) (mg)</t>
-  </si>
-  <si>
-    <t>Niacin (vitamin B3) (mg)</t>
-  </si>
-  <si>
-    <t>Pantothenic Acid (mg)</t>
-  </si>
-  <si>
-    <t>Vitamin B-6 (pyridoxine, pyridoxyl, &amp; pyridoxamine) (mg)</t>
-  </si>
-  <si>
-    <t>Total Folate (mcg)</t>
-  </si>
-  <si>
-    <t>Vitamin B-12 (cobalamin) (mcg)</t>
   </si>
   <si>
     <t>Calcium (mg)</t>
@@ -285,9 +246,6 @@
   </si>
   <si>
     <t>Synthetic Folate (folic acid) (mcg)</t>
-  </si>
-  <si>
-    <t>Total Vitamin A Activity (Retinol Activity Equivalents) (mcg)</t>
   </si>
   <si>
     <t>Energy (kj)</t>
@@ -920,7 +878,49 @@
     <t>pds</t>
   </si>
   <si>
-    <t>CHO (g)</t>
+    <t>Protein (g)</t>
+  </si>
+  <si>
+    <t>Carbohydrate (g)</t>
+  </si>
+  <si>
+    <t>Fat (g)</t>
+  </si>
+  <si>
+    <t>Vitamin A (Retinol) (mcg)</t>
+  </si>
+  <si>
+    <t>Vitamin D (mcg)</t>
+  </si>
+  <si>
+    <t>Vitamin E (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin K (mcg)</t>
+  </si>
+  <si>
+    <t>Vitamin C (Ascorbic acid) (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B1 (Thiamin) (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B2 (Riboflavin) (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B3 (Niacin) (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B6 (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B12 (Cobalamin) (mcg)</t>
+  </si>
+  <si>
+    <t>Vitamin B5 (Pantothenic acid) (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B9 (Folate) (mcg)</t>
   </si>
 </sst>
 </file>
@@ -1309,187 +1309,187 @@
   <dimension ref="A1:GI86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="1" max="2" width="47.625" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="34.83203125" customWidth="1"/>
-    <col min="13" max="13" width="41.33203125" customWidth="1"/>
-    <col min="14" max="14" width="37.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="14.625" customWidth="1"/>
+    <col min="12" max="12" width="34.875" customWidth="1"/>
+    <col min="13" max="13" width="41.375" customWidth="1"/>
+    <col min="14" max="14" width="37.625" customWidth="1"/>
+    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
+    <col min="17" max="17" width="10.125" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="10.1640625" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" customWidth="1"/>
-    <col min="24" max="24" width="23.1640625" customWidth="1"/>
-    <col min="25" max="25" width="9.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.125" customWidth="1"/>
+    <col min="21" max="21" width="9.125" customWidth="1"/>
+    <col min="22" max="22" width="19.625" customWidth="1"/>
+    <col min="23" max="23" width="21.625" customWidth="1"/>
+    <col min="24" max="24" width="23.125" customWidth="1"/>
+    <col min="25" max="25" width="9.625" customWidth="1"/>
     <col min="26" max="26" width="45.5" customWidth="1"/>
-    <col min="27" max="27" width="29.1640625" customWidth="1"/>
-    <col min="28" max="28" width="12.1640625" customWidth="1"/>
-    <col min="29" max="29" width="14.6640625" customWidth="1"/>
+    <col min="27" max="27" width="29.125" customWidth="1"/>
+    <col min="28" max="28" width="12.125" customWidth="1"/>
+    <col min="29" max="29" width="14.625" customWidth="1"/>
     <col min="30" max="30" width="27.5" customWidth="1"/>
     <col min="31" max="31" width="32" customWidth="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="34" width="17.1640625" customWidth="1"/>
-    <col min="35" max="35" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="14.6640625" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" customWidth="1"/>
-    <col min="40" max="40" width="25.6640625" customWidth="1"/>
-    <col min="41" max="41" width="33.33203125" customWidth="1"/>
-    <col min="42" max="42" width="16.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16.625" customWidth="1"/>
+    <col min="33" max="34" width="17.125" customWidth="1"/>
+    <col min="35" max="35" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="14.625" customWidth="1"/>
+    <col min="39" max="39" width="26.375" customWidth="1"/>
+    <col min="40" max="40" width="25.625" customWidth="1"/>
+    <col min="41" max="41" width="33.375" customWidth="1"/>
+    <col min="42" max="42" width="16.375" customWidth="1"/>
     <col min="43" max="43" width="16.5" customWidth="1"/>
-    <col min="44" max="44" width="11.6640625" customWidth="1"/>
+    <col min="44" max="44" width="11.625" customWidth="1"/>
     <col min="45" max="45" width="15.5" customWidth="1"/>
-    <col min="46" max="46" width="15.1640625" customWidth="1"/>
-    <col min="47" max="48" width="8.6640625" customWidth="1"/>
-    <col min="49" max="49" width="11.33203125" customWidth="1"/>
-    <col min="50" max="50" width="14.1640625" customWidth="1"/>
-    <col min="51" max="51" width="11.6640625" customWidth="1"/>
-    <col min="52" max="52" width="14.1640625" customWidth="1"/>
+    <col min="46" max="46" width="15.125" customWidth="1"/>
+    <col min="47" max="48" width="8.625" customWidth="1"/>
+    <col min="49" max="49" width="11.375" customWidth="1"/>
+    <col min="50" max="50" width="14.125" customWidth="1"/>
+    <col min="51" max="51" width="11.625" customWidth="1"/>
+    <col min="52" max="52" width="14.125" customWidth="1"/>
     <col min="53" max="53" width="22" customWidth="1"/>
-    <col min="54" max="54" width="22.1640625" customWidth="1"/>
+    <col min="54" max="54" width="22.125" customWidth="1"/>
     <col min="55" max="55" width="22.5" customWidth="1"/>
     <col min="56" max="56" width="22" customWidth="1"/>
-    <col min="57" max="57" width="21.6640625" customWidth="1"/>
-    <col min="58" max="59" width="23.6640625" customWidth="1"/>
-    <col min="60" max="60" width="24.33203125" customWidth="1"/>
+    <col min="57" max="57" width="21.625" customWidth="1"/>
+    <col min="58" max="59" width="23.625" customWidth="1"/>
+    <col min="60" max="60" width="24.375" customWidth="1"/>
     <col min="61" max="61" width="22.5" customWidth="1"/>
-    <col min="62" max="62" width="24.6640625" customWidth="1"/>
-    <col min="63" max="63" width="23.6640625" customWidth="1"/>
-    <col min="64" max="64" width="28.33203125" customWidth="1"/>
+    <col min="62" max="62" width="24.625" customWidth="1"/>
+    <col min="63" max="63" width="23.625" customWidth="1"/>
+    <col min="64" max="64" width="28.375" customWidth="1"/>
     <col min="65" max="65" width="28.5" customWidth="1"/>
-    <col min="66" max="66" width="22.6640625" customWidth="1"/>
-    <col min="67" max="67" width="26.1640625" customWidth="1"/>
+    <col min="66" max="66" width="22.625" customWidth="1"/>
+    <col min="67" max="67" width="26.125" customWidth="1"/>
     <col min="68" max="68" width="24" customWidth="1"/>
-    <col min="69" max="69" width="24.33203125" customWidth="1"/>
-    <col min="70" max="70" width="25.6640625" customWidth="1"/>
+    <col min="69" max="69" width="24.375" customWidth="1"/>
+    <col min="70" max="70" width="25.625" customWidth="1"/>
     <col min="71" max="71" width="26" customWidth="1"/>
-    <col min="72" max="72" width="28.33203125" customWidth="1"/>
-    <col min="73" max="73" width="38.6640625" customWidth="1"/>
-    <col min="74" max="74" width="39.6640625" customWidth="1"/>
-    <col min="75" max="75" width="38.6640625" customWidth="1"/>
-    <col min="76" max="76" width="13.6640625" customWidth="1"/>
-    <col min="77" max="77" width="12.33203125" customWidth="1"/>
-    <col min="78" max="78" width="12.1640625" customWidth="1"/>
-    <col min="79" max="79" width="10.1640625" customWidth="1"/>
-    <col min="80" max="80" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="13.6640625" customWidth="1"/>
-    <col min="82" max="82" width="9.6640625" customWidth="1"/>
-    <col min="83" max="83" width="15.6640625" customWidth="1"/>
-    <col min="84" max="84" width="10.6640625" customWidth="1"/>
-    <col min="85" max="85" width="8.6640625" customWidth="1"/>
-    <col min="86" max="86" width="10.6640625" customWidth="1"/>
-    <col min="87" max="87" width="11.1640625" customWidth="1"/>
-    <col min="88" max="88" width="10.1640625" customWidth="1"/>
+    <col min="72" max="72" width="28.375" customWidth="1"/>
+    <col min="73" max="73" width="38.625" customWidth="1"/>
+    <col min="74" max="74" width="39.625" customWidth="1"/>
+    <col min="75" max="75" width="38.625" customWidth="1"/>
+    <col min="76" max="76" width="13.625" customWidth="1"/>
+    <col min="77" max="77" width="12.375" customWidth="1"/>
+    <col min="78" max="78" width="12.125" customWidth="1"/>
+    <col min="79" max="79" width="10.125" customWidth="1"/>
+    <col min="80" max="80" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.625" customWidth="1"/>
+    <col min="82" max="82" width="9.625" customWidth="1"/>
+    <col min="83" max="83" width="15.625" customWidth="1"/>
+    <col min="84" max="84" width="10.625" customWidth="1"/>
+    <col min="85" max="85" width="8.625" customWidth="1"/>
+    <col min="86" max="86" width="10.625" customWidth="1"/>
+    <col min="87" max="87" width="11.125" customWidth="1"/>
+    <col min="88" max="88" width="10.125" customWidth="1"/>
     <col min="89" max="89" width="15" customWidth="1"/>
-    <col min="90" max="90" width="49.33203125" customWidth="1"/>
-    <col min="91" max="91" width="9.6640625" customWidth="1"/>
-    <col min="92" max="92" width="22.6640625" customWidth="1"/>
+    <col min="90" max="90" width="49.375" customWidth="1"/>
+    <col min="91" max="91" width="9.625" customWidth="1"/>
+    <col min="92" max="92" width="22.625" customWidth="1"/>
     <col min="93" max="93" width="9" customWidth="1"/>
-    <col min="94" max="94" width="14.6640625" customWidth="1"/>
-    <col min="95" max="95" width="13.6640625" customWidth="1"/>
-    <col min="96" max="96" width="12.1640625" customWidth="1"/>
+    <col min="94" max="94" width="14.625" customWidth="1"/>
+    <col min="95" max="95" width="13.625" customWidth="1"/>
+    <col min="96" max="96" width="12.125" customWidth="1"/>
     <col min="97" max="97" width="15" customWidth="1"/>
-    <col min="98" max="98" width="14.6640625" customWidth="1"/>
-    <col min="99" max="99" width="20.6640625" customWidth="1"/>
+    <col min="98" max="98" width="14.625" customWidth="1"/>
+    <col min="99" max="99" width="20.625" customWidth="1"/>
     <col min="100" max="100" width="19" customWidth="1"/>
-    <col min="101" max="101" width="6.6640625" customWidth="1"/>
+    <col min="101" max="101" width="6.625" customWidth="1"/>
     <col min="102" max="102" width="9" customWidth="1"/>
     <col min="103" max="103" width="17.5" customWidth="1"/>
-    <col min="104" max="104" width="26.6640625" customWidth="1"/>
-    <col min="105" max="105" width="21.33203125" customWidth="1"/>
+    <col min="104" max="104" width="26.625" customWidth="1"/>
+    <col min="105" max="105" width="21.375" customWidth="1"/>
     <col min="106" max="106" width="21.5" customWidth="1"/>
     <col min="107" max="107" width="18" customWidth="1"/>
     <col min="108" max="108" width="20" customWidth="1"/>
-    <col min="109" max="109" width="19.33203125" customWidth="1"/>
-    <col min="110" max="110" width="35.33203125" customWidth="1"/>
-    <col min="111" max="111" width="36.6640625" customWidth="1"/>
-    <col min="112" max="112" width="45.6640625" customWidth="1"/>
-    <col min="113" max="113" width="36.1640625" customWidth="1"/>
+    <col min="109" max="109" width="19.375" customWidth="1"/>
+    <col min="110" max="110" width="35.375" customWidth="1"/>
+    <col min="111" max="111" width="36.625" customWidth="1"/>
+    <col min="112" max="112" width="45.625" customWidth="1"/>
+    <col min="113" max="113" width="36.125" customWidth="1"/>
     <col min="114" max="114" width="39" customWidth="1"/>
     <col min="115" max="115" width="36.5" customWidth="1"/>
-    <col min="116" max="116" width="31.1640625" customWidth="1"/>
-    <col min="117" max="117" width="42.1640625" customWidth="1"/>
-    <col min="118" max="118" width="43.33203125" customWidth="1"/>
-    <col min="119" max="119" width="46.6640625" customWidth="1"/>
-    <col min="120" max="120" width="23.33203125" customWidth="1"/>
-    <col min="121" max="121" width="14.33203125" customWidth="1"/>
+    <col min="116" max="116" width="31.125" customWidth="1"/>
+    <col min="117" max="117" width="42.125" customWidth="1"/>
+    <col min="118" max="118" width="43.375" customWidth="1"/>
+    <col min="119" max="119" width="46.625" customWidth="1"/>
+    <col min="120" max="120" width="23.375" customWidth="1"/>
+    <col min="121" max="121" width="14.375" customWidth="1"/>
     <col min="122" max="122" width="29" customWidth="1"/>
-    <col min="123" max="123" width="30.1640625" customWidth="1"/>
+    <col min="123" max="123" width="30.125" customWidth="1"/>
     <col min="124" max="124" width="30" customWidth="1"/>
-    <col min="125" max="125" width="53.1640625" customWidth="1"/>
+    <col min="125" max="125" width="53.125" customWidth="1"/>
     <col min="126" max="126" width="10" customWidth="1"/>
-    <col min="127" max="127" width="21.33203125" customWidth="1"/>
-    <col min="128" max="128" width="14.1640625" customWidth="1"/>
+    <col min="127" max="127" width="21.375" customWidth="1"/>
+    <col min="128" max="128" width="14.125" customWidth="1"/>
     <col min="129" max="129" width="21.5" customWidth="1"/>
-    <col min="130" max="130" width="15.1640625" customWidth="1"/>
+    <col min="130" max="130" width="15.125" customWidth="1"/>
     <col min="131" max="131" width="12.5" customWidth="1"/>
-    <col min="132" max="132" width="28.1640625" customWidth="1"/>
-    <col min="133" max="133" width="29.6640625" customWidth="1"/>
+    <col min="132" max="132" width="28.125" customWidth="1"/>
+    <col min="133" max="133" width="29.625" customWidth="1"/>
     <col min="134" max="134" width="12.5" customWidth="1"/>
-    <col min="135" max="135" width="13.33203125" customWidth="1"/>
-    <col min="136" max="136" width="12.6640625" customWidth="1"/>
-    <col min="137" max="137" width="15.1640625" customWidth="1"/>
-    <col min="138" max="138" width="15.6640625" customWidth="1"/>
-    <col min="139" max="139" width="17.6640625" customWidth="1"/>
-    <col min="140" max="140" width="40.6640625" customWidth="1"/>
-    <col min="141" max="141" width="24.6640625" customWidth="1"/>
+    <col min="135" max="135" width="13.375" customWidth="1"/>
+    <col min="136" max="136" width="12.625" customWidth="1"/>
+    <col min="137" max="137" width="15.125" customWidth="1"/>
+    <col min="138" max="138" width="15.625" customWidth="1"/>
+    <col min="139" max="139" width="17.625" customWidth="1"/>
+    <col min="140" max="140" width="40.625" customWidth="1"/>
+    <col min="141" max="141" width="24.625" customWidth="1"/>
     <col min="142" max="142" width="13.5" customWidth="1"/>
-    <col min="143" max="143" width="24.1640625" customWidth="1"/>
+    <col min="143" max="143" width="24.125" customWidth="1"/>
     <col min="144" max="144" width="31" customWidth="1"/>
-    <col min="145" max="145" width="29.6640625" customWidth="1"/>
+    <col min="145" max="145" width="29.625" customWidth="1"/>
     <col min="146" max="146" width="30.5" customWidth="1"/>
     <col min="147" max="147" width="29" customWidth="1"/>
-    <col min="148" max="150" width="11.6640625" customWidth="1"/>
+    <col min="148" max="150" width="11.625" customWidth="1"/>
     <col min="151" max="151" width="10" customWidth="1"/>
-    <col min="152" max="152" width="9.6640625" customWidth="1"/>
+    <col min="152" max="152" width="9.625" customWidth="1"/>
     <col min="153" max="153" width="10" customWidth="1"/>
     <col min="154" max="154" width="10.5" customWidth="1"/>
     <col min="155" max="155" width="11.5" customWidth="1"/>
-    <col min="156" max="156" width="9.1640625" customWidth="1"/>
+    <col min="156" max="156" width="9.125" customWidth="1"/>
     <col min="157" max="157" width="10.5" customWidth="1"/>
-    <col min="158" max="158" width="9.1640625" customWidth="1"/>
-    <col min="159" max="159" width="11.1640625" customWidth="1"/>
-    <col min="160" max="160" width="39.1640625" customWidth="1"/>
-    <col min="161" max="161" width="19.1640625" customWidth="1"/>
-    <col min="162" max="162" width="20.1640625" customWidth="1"/>
+    <col min="158" max="158" width="9.125" customWidth="1"/>
+    <col min="159" max="159" width="11.125" customWidth="1"/>
+    <col min="160" max="160" width="39.125" customWidth="1"/>
+    <col min="161" max="161" width="19.125" customWidth="1"/>
+    <col min="162" max="162" width="20.125" customWidth="1"/>
     <col min="163" max="163" width="13" customWidth="1"/>
     <col min="164" max="164" width="29.5" customWidth="1"/>
-    <col min="165" max="165" width="30.1640625" customWidth="1"/>
-    <col min="166" max="166" width="30.6640625" customWidth="1"/>
+    <col min="165" max="165" width="30.125" customWidth="1"/>
+    <col min="166" max="166" width="30.625" customWidth="1"/>
     <col min="167" max="167" width="29" customWidth="1"/>
-    <col min="168" max="168" width="30.33203125" customWidth="1"/>
-    <col min="169" max="169" width="31.1640625" customWidth="1"/>
-    <col min="170" max="170" width="39.6640625" customWidth="1"/>
-    <col min="171" max="171" width="11.6640625" customWidth="1"/>
-    <col min="172" max="191" width="8.6640625" customWidth="1"/>
+    <col min="168" max="168" width="30.375" customWidth="1"/>
+    <col min="169" max="169" width="31.125" customWidth="1"/>
+    <col min="170" max="170" width="39.625" customWidth="1"/>
+    <col min="171" max="171" width="11.625" customWidth="1"/>
+    <col min="172" max="191" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1498,379 +1498,379 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AR1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="CM1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="DM1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="DZ1" s="2"/>
       <c r="EA1" s="2"/>
@@ -1935,12 +1935,12 @@
       <c r="GH1" s="3"/>
       <c r="GI1" s="3"/>
     </row>
-    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C2" s="2">
         <v>1.04</v>
@@ -2386,12 +2386,12 @@
       <c r="GH2" s="4"/>
       <c r="GI2" s="4"/>
     </row>
-    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2">
         <v>30.7</v>
@@ -2837,12 +2837,12 @@
       <c r="GH3" s="4"/>
       <c r="GI3" s="4"/>
     </row>
-    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3288,12 +3288,12 @@
       <c r="GH4" s="4"/>
       <c r="GI4" s="4"/>
     </row>
-    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C5" s="2">
         <v>29.6</v>
@@ -3739,12 +3739,12 @@
       <c r="GH5" s="4"/>
       <c r="GI5" s="4"/>
     </row>
-    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="C6" s="2">
         <v>30.5</v>
@@ -4190,12 +4190,12 @@
       <c r="GH6" s="4"/>
       <c r="GI6" s="4"/>
     </row>
-    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2">
         <v>31.3</v>
@@ -4641,12 +4641,12 @@
       <c r="GH7" s="4"/>
       <c r="GI7" s="4"/>
     </row>
-    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="C8" s="2">
         <v>30.2</v>
@@ -5092,12 +5092,12 @@
       <c r="GH8" s="4"/>
       <c r="GI8" s="4"/>
     </row>
-    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C9" s="2">
         <v>25.2</v>
@@ -5543,12 +5543,12 @@
       <c r="GH9" s="4"/>
       <c r="GI9" s="4"/>
     </row>
-    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="C10" s="2">
         <v>29.5</v>
@@ -5994,12 +5994,12 @@
       <c r="GH10" s="4"/>
       <c r="GI10" s="4"/>
     </row>
-    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C11" s="2">
         <v>113.4</v>
@@ -6445,12 +6445,12 @@
       <c r="GH11" s="4"/>
       <c r="GI11" s="4"/>
     </row>
-    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C12" s="2">
         <v>28.4</v>
@@ -6896,12 +6896,12 @@
       <c r="GH12" s="4"/>
       <c r="GI12" s="4"/>
     </row>
-    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="C13" s="2">
         <v>31.1</v>
@@ -7347,12 +7347,12 @@
       <c r="GH13" s="4"/>
       <c r="GI13" s="4"/>
     </row>
-    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C14" s="2">
         <v>31.3</v>
@@ -7798,12 +7798,12 @@
       <c r="GH14" s="4"/>
       <c r="GI14" s="4"/>
     </row>
-    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C15" s="2">
         <v>30.1</v>
@@ -8249,12 +8249,12 @@
       <c r="GH15" s="4"/>
       <c r="GI15" s="4"/>
     </row>
-    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="C16" s="2">
         <v>29</v>
@@ -8700,12 +8700,12 @@
       <c r="GH16" s="4"/>
       <c r="GI16" s="4"/>
     </row>
-    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C17" s="2">
         <v>28.4</v>
@@ -9151,12 +9151,12 @@
       <c r="GH17" s="4"/>
       <c r="GI17" s="4"/>
     </row>
-    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C18" s="2">
         <v>30.7</v>
@@ -9602,12 +9602,12 @@
       <c r="GH18" s="4"/>
       <c r="GI18" s="4"/>
     </row>
-    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="C19" s="2">
         <v>30.5</v>
@@ -10053,12 +10053,12 @@
       <c r="GH19" s="4"/>
       <c r="GI19" s="4"/>
     </row>
-    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C20" s="2">
         <v>30.7</v>
@@ -10504,12 +10504,12 @@
       <c r="GH20" s="4"/>
       <c r="GI20" s="4"/>
     </row>
-    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C21" s="2">
         <v>28.4</v>
@@ -10955,12 +10955,12 @@
       <c r="GH21" s="4"/>
       <c r="GI21" s="4"/>
     </row>
-    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C22" s="2">
         <v>28.4</v>
@@ -11406,12 +11406,12 @@
       <c r="GH22" s="4"/>
       <c r="GI22" s="4"/>
     </row>
-    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="C23" s="2">
         <v>4.2</v>
@@ -11857,12 +11857,12 @@
       <c r="GH23" s="4"/>
       <c r="GI23" s="4"/>
     </row>
-    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C24" s="2">
         <v>28.4</v>
@@ -12308,12 +12308,12 @@
       <c r="GH24" s="4"/>
       <c r="GI24" s="4"/>
     </row>
-    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C25" s="2">
         <v>28.4</v>
@@ -12759,12 +12759,12 @@
       <c r="GH25" s="4"/>
       <c r="GI25" s="4"/>
     </row>
-    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="C26" s="2">
         <v>28.4</v>
@@ -13210,12 +13210,12 @@
       <c r="GH26" s="4"/>
       <c r="GI26" s="4"/>
     </row>
-    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C27" s="2">
         <v>28.4</v>
@@ -13661,12 +13661,12 @@
       <c r="GH27" s="4"/>
       <c r="GI27" s="4"/>
     </row>
-    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C28" s="2">
         <v>35.1</v>
@@ -14112,12 +14112,12 @@
       <c r="GH28" s="4"/>
       <c r="GI28" s="4"/>
     </row>
-    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C29" s="2">
         <v>40.299999999999997</v>
@@ -14563,12 +14563,12 @@
       <c r="GH29" s="4"/>
       <c r="GI29" s="4"/>
     </row>
-    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C30" s="2">
         <v>45.8</v>
@@ -15014,12 +15014,12 @@
       <c r="GH30" s="4"/>
       <c r="GI30" s="4"/>
     </row>
-    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C31" s="2">
         <v>49.7</v>
@@ -15465,12 +15465,12 @@
       <c r="GH31" s="4"/>
       <c r="GI31" s="4"/>
     </row>
-    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C32" s="2">
         <v>4.5999999999999996</v>
@@ -15916,12 +15916,12 @@
       <c r="GH32" s="4"/>
       <c r="GI32" s="4"/>
     </row>
-    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -16367,12 +16367,12 @@
       <c r="GH33" s="4"/>
       <c r="GI33" s="4"/>
     </row>
-    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="C34" s="2">
         <v>91.9</v>
@@ -16818,12 +16818,12 @@
       <c r="GH34" s="4"/>
       <c r="GI34" s="4"/>
     </row>
-    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C35" s="2">
         <v>28.4</v>
@@ -17269,12 +17269,12 @@
       <c r="GH35" s="4"/>
       <c r="GI35" s="4"/>
     </row>
-    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C36" s="2">
         <v>28.4</v>
@@ -17720,12 +17720,12 @@
       <c r="GH36" s="4"/>
       <c r="GI36" s="4"/>
     </row>
-    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C37" s="2">
         <v>30</v>
@@ -18171,12 +18171,12 @@
       <c r="GH37" s="4"/>
       <c r="GI37" s="4"/>
     </row>
-    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C38" s="2">
         <v>28.4</v>
@@ -18622,12 +18622,12 @@
       <c r="GH38" s="4"/>
       <c r="GI38" s="4"/>
     </row>
-    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="C39" s="2">
         <v>28.4</v>
@@ -19073,12 +19073,12 @@
       <c r="GH39" s="4"/>
       <c r="GI39" s="4"/>
     </row>
-    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C40" s="2">
         <v>28.4</v>
@@ -19524,12 +19524,12 @@
       <c r="GH40" s="4"/>
       <c r="GI40" s="4"/>
     </row>
-    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C41" s="2">
         <v>28.4</v>
@@ -19975,12 +19975,12 @@
       <c r="GH41" s="4"/>
       <c r="GI41" s="4"/>
     </row>
-    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C42" s="2">
         <v>28.4</v>
@@ -20426,12 +20426,12 @@
       <c r="GH42" s="4"/>
       <c r="GI42" s="4"/>
     </row>
-    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C43" s="2">
         <v>28.4</v>
@@ -20877,12 +20877,12 @@
       <c r="GH43" s="4"/>
       <c r="GI43" s="4"/>
     </row>
-    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C44" s="2">
         <v>28.4</v>
@@ -21328,12 +21328,12 @@
       <c r="GH44" s="4"/>
       <c r="GI44" s="4"/>
     </row>
-    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C45" s="2">
         <v>28.4</v>
@@ -21779,12 +21779,12 @@
       <c r="GH45" s="4"/>
       <c r="GI45" s="4"/>
     </row>
-    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C46" s="2">
         <v>28.4</v>
@@ -22230,12 +22230,12 @@
       <c r="GH46" s="4"/>
       <c r="GI46" s="4"/>
     </row>
-    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C47" s="2">
         <v>28.4</v>
@@ -22681,12 +22681,12 @@
       <c r="GH47" s="4"/>
       <c r="GI47" s="4"/>
     </row>
-    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C48" s="2">
         <v>28.4</v>
@@ -23132,12 +23132,12 @@
       <c r="GH48" s="4"/>
       <c r="GI48" s="4"/>
     </row>
-    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C49" s="2">
         <v>28.4</v>
@@ -23583,12 +23583,12 @@
       <c r="GH49" s="4"/>
       <c r="GI49" s="4"/>
     </row>
-    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C50" s="2">
         <v>28.4</v>
@@ -24034,12 +24034,12 @@
       <c r="GH50" s="4"/>
       <c r="GI50" s="4"/>
     </row>
-    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C51" s="2">
         <v>28.4</v>
@@ -24485,12 +24485,12 @@
       <c r="GH51" s="4"/>
       <c r="GI51" s="4"/>
     </row>
-    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C52" s="2">
         <v>28.4</v>
@@ -24936,12 +24936,12 @@
       <c r="GH52" s="4"/>
       <c r="GI52" s="4"/>
     </row>
-    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C53" s="2">
         <v>28.4</v>
@@ -25387,12 +25387,12 @@
       <c r="GH53" s="4"/>
       <c r="GI53" s="4"/>
     </row>
-    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C54" s="2">
         <v>28.4</v>
@@ -25838,12 +25838,12 @@
       <c r="GH54" s="4"/>
       <c r="GI54" s="4"/>
     </row>
-    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C55" s="2">
         <v>28.4</v>
@@ -26289,12 +26289,12 @@
       <c r="GH55" s="4"/>
       <c r="GI55" s="4"/>
     </row>
-    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C56" s="2">
         <v>28.4</v>
@@ -26740,12 +26740,12 @@
       <c r="GH56" s="4"/>
       <c r="GI56" s="4"/>
     </row>
-    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C57" s="2">
         <v>28.4</v>
@@ -27191,12 +27191,12 @@
       <c r="GH57" s="4"/>
       <c r="GI57" s="4"/>
     </row>
-    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C58" s="2">
         <v>28.4</v>
@@ -27642,12 +27642,12 @@
       <c r="GH58" s="4"/>
       <c r="GI58" s="4"/>
     </row>
-    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C59" s="2">
         <v>28.4</v>
@@ -28093,12 +28093,12 @@
       <c r="GH59" s="4"/>
       <c r="GI59" s="4"/>
     </row>
-    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C60" s="2">
         <v>28.4</v>
@@ -28544,12 +28544,12 @@
       <c r="GH60" s="2"/>
       <c r="GI60" s="2"/>
     </row>
-    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C61" s="2">
         <v>28.4</v>
@@ -28995,12 +28995,12 @@
       <c r="GH61" s="4"/>
       <c r="GI61" s="4"/>
     </row>
-    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C62" s="2">
         <v>28.4</v>
@@ -29446,12 +29446,12 @@
       <c r="GH62" s="4"/>
       <c r="GI62" s="4"/>
     </row>
-    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C63" s="2">
         <v>28.4</v>
@@ -29897,12 +29897,12 @@
       <c r="GH63" s="4"/>
       <c r="GI63" s="4"/>
     </row>
-    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="C64" s="2">
         <v>28.4</v>
@@ -30348,12 +30348,12 @@
       <c r="GH64" s="4"/>
       <c r="GI64" s="4"/>
     </row>
-    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C65" s="2">
         <v>28.4</v>
@@ -30799,12 +30799,12 @@
       <c r="GH65" s="4"/>
       <c r="GI65" s="4"/>
     </row>
-    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C66" s="2">
         <v>28.4</v>
@@ -31250,12 +31250,12 @@
       <c r="GH66" s="4"/>
       <c r="GI66" s="4"/>
     </row>
-    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C67" s="2">
         <v>28.4</v>
@@ -31701,12 +31701,12 @@
       <c r="GH67" s="4"/>
       <c r="GI67" s="4"/>
     </row>
-    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C68" s="2">
         <v>28.4</v>
@@ -32152,12 +32152,12 @@
       <c r="GH68" s="4"/>
       <c r="GI68" s="4"/>
     </row>
-    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C69" s="2">
         <v>28.4</v>
@@ -32603,12 +32603,12 @@
       <c r="GH69" s="4"/>
       <c r="GI69" s="4"/>
     </row>
-    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C70" s="2">
         <v>28.4</v>
@@ -33054,12 +33054,12 @@
       <c r="GH70" s="4"/>
       <c r="GI70" s="4"/>
     </row>
-    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C71" s="2">
         <v>28.4</v>
@@ -33505,12 +33505,12 @@
       <c r="GH71" s="4"/>
       <c r="GI71" s="4"/>
     </row>
-    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="C72" s="2">
         <v>28.4</v>
@@ -33956,12 +33956,12 @@
       <c r="GH72" s="4"/>
       <c r="GI72" s="4"/>
     </row>
-    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C73" s="2">
         <v>28.4</v>
@@ -34407,12 +34407,12 @@
       <c r="GH73" s="4"/>
       <c r="GI73" s="4"/>
     </row>
-    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C74" s="2">
         <v>28.4</v>
@@ -34858,12 +34858,12 @@
       <c r="GH74" s="4"/>
       <c r="GI74" s="4"/>
     </row>
-    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C75" s="2">
         <v>28.4</v>
@@ -35309,12 +35309,12 @@
       <c r="GH75" s="4"/>
       <c r="GI75" s="4"/>
     </row>
-    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="C76" s="2">
         <v>28.4</v>
@@ -35760,12 +35760,12 @@
       <c r="GH76" s="4"/>
       <c r="GI76" s="4"/>
     </row>
-    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C77" s="2">
         <v>43.3</v>
@@ -36211,12 +36211,12 @@
       <c r="GH77" s="4"/>
       <c r="GI77" s="4"/>
     </row>
-    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C78" s="2">
         <v>28.4</v>
@@ -36662,12 +36662,12 @@
       <c r="GH78" s="4"/>
       <c r="GI78" s="4"/>
     </row>
-    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C79" s="2">
         <v>26.2</v>
@@ -37113,12 +37113,12 @@
       <c r="GH79" s="4"/>
       <c r="GI79" s="4"/>
     </row>
-    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C80" s="2">
         <v>59.4</v>
@@ -37564,12 +37564,12 @@
       <c r="GH80" s="4"/>
       <c r="GI80" s="4"/>
     </row>
-    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C81" s="2">
         <v>10.8</v>
@@ -38015,12 +38015,12 @@
       <c r="GH81" s="4"/>
       <c r="GI81" s="4"/>
     </row>
-    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C82" s="2">
         <v>6.8</v>
@@ -38466,12 +38466,12 @@
       <c r="GH82" s="4"/>
       <c r="GI82" s="4"/>
     </row>
-    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C83" s="2">
         <v>28.4</v>
@@ -38917,12 +38917,12 @@
       <c r="GH83" s="4"/>
       <c r="GI83" s="4"/>
     </row>
-    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C84" s="2">
         <v>4.7</v>
@@ -39368,12 +39368,12 @@
       <c r="GH84" s="4"/>
       <c r="GI84" s="4"/>
     </row>
-    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C85" s="6">
         <v>4.5</v>
@@ -39757,12 +39757,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:191" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="C86" s="2">
         <v>31</v>

</xml_diff>